<commit_message>
Change '_' to '-' in Excel metadata
Close #5
</commit_message>
<xml_diff>
--- a/tests/testthat/fixtures/metadata/metadata_BEXLTALL.xlsx
+++ b/tests/testthat/fixtures/metadata/metadata_BEXLTALL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/672a29ec829a16e8/Dokumenter/GitHub/ProjCore/px/data-raw/metadata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johan Ejstrud\Dropbox\repo\pxmake\tests\testthat\fixtures\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{79CCC2D3-1A8E-44B3-94BD-6033C059658E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB47A784-CBF9-4162-97DF-259F84945E4E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74036D84-B5C2-4940-99CB-0AEFBCCE56CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="17265" windowHeight="31800" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables_MD" sheetId="1" r:id="rId1"/>
@@ -672,27 +672,15 @@
     <t>Statistics Greenland</t>
   </si>
   <si>
-    <t>SUBJECT_CODE</t>
-  </si>
-  <si>
     <t>BE</t>
   </si>
   <si>
-    <t>SUBJECT_AREA_da</t>
-  </si>
-  <si>
     <t>Befolkning</t>
   </si>
   <si>
-    <t>SUBJECT_AREA_en</t>
-  </si>
-  <si>
     <t>Population</t>
   </si>
   <si>
-    <t>SUBJECT_AREA_kl</t>
-  </si>
-  <si>
     <t>Innuttaasut</t>
   </si>
   <si>
@@ -705,24 +693,15 @@
     <t>DESCRIPTION_kl</t>
   </si>
   <si>
-    <t>CREATION_DATE</t>
-  </si>
-  <si>
     <t>20190124 09:00</t>
   </si>
   <si>
-    <t>UPDATE_FREQUENCY</t>
-  </si>
-  <si>
     <t>Annually</t>
   </si>
   <si>
     <t>20220222 09:00</t>
   </si>
   <si>
-    <t>NEXT_UPDATE</t>
-  </si>
-  <si>
     <t>LINK_da</t>
   </si>
   <si>
@@ -828,9 +807,6 @@
     <t>CHARSET</t>
   </si>
   <si>
-    <t>AXIS_VERSION</t>
-  </si>
-  <si>
     <t>LANGUAGE</t>
   </si>
   <si>
@@ -849,9 +825,6 @@
     <t>BEXLTALL</t>
   </si>
   <si>
-    <t>LAST_UPDATED</t>
-  </si>
-  <si>
     <t>DECIMALS</t>
   </si>
   <si>
@@ -877,6 +850,33 @@
   </si>
   <si>
     <t>ANSI</t>
+  </si>
+  <si>
+    <t>AXIS-VERSION</t>
+  </si>
+  <si>
+    <t>SUBJECT-CODE</t>
+  </si>
+  <si>
+    <t>SUBJECT-AREA_da</t>
+  </si>
+  <si>
+    <t>SUBJECT-AREA_en</t>
+  </si>
+  <si>
+    <t>SUBJECT-AREA_kl</t>
+  </si>
+  <si>
+    <t>CREATION-DATE</t>
+  </si>
+  <si>
+    <t>UPDATE-FREQUENCY</t>
+  </si>
+  <si>
+    <t>LAST-UPDATED</t>
+  </si>
+  <si>
+    <t>NEXT-UPDATE</t>
   </si>
 </sst>
 </file>
@@ -947,7 +947,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1273,25 +1273,25 @@
       <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="12.73046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.86328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.86328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.3984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.73046875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.86328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.59765625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.86328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.265625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1338,7 +1338,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -1358,7 +1358,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -1387,7 +1387,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -1395,7 +1395,7 @@
         <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
       <c r="D4" t="s">
         <v>29</v>
@@ -1416,7 +1416,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -1454,15 +1454,15 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>42</v>
       </c>
       <c r="B6" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="C6" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="D6" t="s">
         <v>43</v>
@@ -1483,7 +1483,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -1491,7 +1491,7 @@
         <v>46</v>
       </c>
       <c r="C7" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="D7" t="s">
         <v>47</v>
@@ -1512,7 +1512,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>50</v>
       </c>
@@ -1541,21 +1541,21 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>193</v>
       </c>
       <c r="C9" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
       <c r="D9" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
       <c r="E9" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
       <c r="F9" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
     </row>
   </sheetData>
@@ -1571,17 +1571,17 @@
       <selection activeCell="D90" sqref="D90"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1604,7 +1604,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>63</v>
       </c>
@@ -1625,7 +1625,7 @@
       </c>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>63</v>
       </c>
@@ -1636,22 +1636,22 @@
         <v>66</v>
       </c>
       <c r="D3" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="E3" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="F3">
         <v>2</v>
       </c>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="C4" t="s">
         <v>67</v>
@@ -1667,12 +1667,12 @@
       </c>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="C5" t="s">
         <v>71</v>
@@ -1688,12 +1688,12 @@
       </c>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="C6" t="s">
         <v>31</v>
@@ -1709,7 +1709,7 @@
       </c>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>76</v>
       </c>
@@ -1730,7 +1730,7 @@
       </c>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>76</v>
       </c>
@@ -1751,7 +1751,7 @@
       </c>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>76</v>
       </c>
@@ -1772,7 +1772,7 @@
       </c>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>76</v>
       </c>
@@ -1793,7 +1793,7 @@
       </c>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>76</v>
       </c>
@@ -1814,7 +1814,7 @@
       </c>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>76</v>
       </c>
@@ -1835,7 +1835,7 @@
       </c>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>76</v>
       </c>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>76</v>
       </c>
@@ -1877,7 +1877,7 @@
       </c>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>76</v>
       </c>
@@ -1898,7 +1898,7 @@
       </c>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>76</v>
       </c>
@@ -1919,7 +1919,7 @@
       </c>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>76</v>
       </c>
@@ -1940,7 +1940,7 @@
       </c>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>76</v>
       </c>
@@ -1961,7 +1961,7 @@
       </c>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>76</v>
       </c>
@@ -1982,7 +1982,7 @@
       </c>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>76</v>
       </c>
@@ -2003,7 +2003,7 @@
       </c>
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>76</v>
       </c>
@@ -2024,7 +2024,7 @@
       </c>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>76</v>
       </c>
@@ -2045,7 +2045,7 @@
       </c>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>76</v>
       </c>
@@ -2066,7 +2066,7 @@
       </c>
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>76</v>
       </c>
@@ -2087,7 +2087,7 @@
       </c>
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>76</v>
       </c>
@@ -2108,7 +2108,7 @@
       </c>
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>76</v>
       </c>
@@ -2129,7 +2129,7 @@
       </c>
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>76</v>
       </c>
@@ -2150,7 +2150,7 @@
       </c>
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>76</v>
       </c>
@@ -2171,7 +2171,7 @@
       </c>
       <c r="G28" s="2"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>76</v>
       </c>
@@ -2192,7 +2192,7 @@
       </c>
       <c r="G29" s="2"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>76</v>
       </c>
@@ -2213,7 +2213,7 @@
       </c>
       <c r="G30" s="2"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>76</v>
       </c>
@@ -2234,7 +2234,7 @@
       </c>
       <c r="G31" s="2"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>76</v>
       </c>
@@ -2255,7 +2255,7 @@
       </c>
       <c r="G32" s="2"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>76</v>
       </c>
@@ -2276,7 +2276,7 @@
       </c>
       <c r="G33" s="2"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>76</v>
       </c>
@@ -2297,7 +2297,7 @@
       </c>
       <c r="G34" s="2"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>76</v>
       </c>
@@ -2318,7 +2318,7 @@
       </c>
       <c r="G35" s="2"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>76</v>
       </c>
@@ -2339,7 +2339,7 @@
       </c>
       <c r="G36" s="2"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>76</v>
       </c>
@@ -2360,7 +2360,7 @@
       </c>
       <c r="G37" s="2"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>76</v>
       </c>
@@ -2381,7 +2381,7 @@
       </c>
       <c r="G38" s="2"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>76</v>
       </c>
@@ -2402,7 +2402,7 @@
       </c>
       <c r="G39" s="2"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>76</v>
       </c>
@@ -2423,7 +2423,7 @@
       </c>
       <c r="G40" s="2"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>76</v>
       </c>
@@ -2444,7 +2444,7 @@
       </c>
       <c r="G41" s="2"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>76</v>
       </c>
@@ -2465,7 +2465,7 @@
       </c>
       <c r="G42" s="2"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>76</v>
       </c>
@@ -2486,7 +2486,7 @@
       </c>
       <c r="G43" s="2"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>76</v>
       </c>
@@ -2507,7 +2507,7 @@
       </c>
       <c r="G44" s="2"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>76</v>
       </c>
@@ -2528,7 +2528,7 @@
       </c>
       <c r="G45" s="2"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>76</v>
       </c>
@@ -2549,7 +2549,7 @@
       </c>
       <c r="G46" s="2"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>76</v>
       </c>
@@ -2570,7 +2570,7 @@
       </c>
       <c r="G47" s="2"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>76</v>
       </c>
@@ -2591,7 +2591,7 @@
       </c>
       <c r="G48" s="2"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>76</v>
       </c>
@@ -2612,7 +2612,7 @@
       </c>
       <c r="G49" s="2"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>76</v>
       </c>
@@ -2633,7 +2633,7 @@
       </c>
       <c r="G50" s="2"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>76</v>
       </c>
@@ -2654,7 +2654,7 @@
       </c>
       <c r="G51" s="2"/>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>76</v>
       </c>
@@ -2675,7 +2675,7 @@
       </c>
       <c r="G52" s="2"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>76</v>
       </c>
@@ -2696,7 +2696,7 @@
       </c>
       <c r="G53" s="2"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>76</v>
       </c>
@@ -2717,7 +2717,7 @@
       </c>
       <c r="G54" s="2"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>76</v>
       </c>
@@ -2738,7 +2738,7 @@
       </c>
       <c r="G55" s="2"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>76</v>
       </c>
@@ -2759,7 +2759,7 @@
       </c>
       <c r="G56" s="2"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>76</v>
       </c>
@@ -2780,7 +2780,7 @@
       </c>
       <c r="G57" s="2"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>76</v>
       </c>
@@ -2801,7 +2801,7 @@
       </c>
       <c r="G58" s="2"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>76</v>
       </c>
@@ -2822,7 +2822,7 @@
       </c>
       <c r="G59" s="2"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>76</v>
       </c>
@@ -2843,7 +2843,7 @@
       </c>
       <c r="G60" s="2"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>76</v>
       </c>
@@ -2864,7 +2864,7 @@
       </c>
       <c r="G61" s="2"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>76</v>
       </c>
@@ -2885,7 +2885,7 @@
       </c>
       <c r="G62" s="2"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>76</v>
       </c>
@@ -2906,7 +2906,7 @@
       </c>
       <c r="G63" s="2"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>76</v>
       </c>
@@ -2927,7 +2927,7 @@
       </c>
       <c r="G64" s="2"/>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>76</v>
       </c>
@@ -2948,7 +2948,7 @@
       </c>
       <c r="G65" s="2"/>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>76</v>
       </c>
@@ -2969,7 +2969,7 @@
       </c>
       <c r="G66" s="2"/>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>76</v>
       </c>
@@ -2990,7 +2990,7 @@
       </c>
       <c r="G67" s="2"/>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>76</v>
       </c>
@@ -3011,7 +3011,7 @@
       </c>
       <c r="G68" s="2"/>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>76</v>
       </c>
@@ -3032,7 +3032,7 @@
       </c>
       <c r="G69" s="2"/>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>76</v>
       </c>
@@ -3053,7 +3053,7 @@
       </c>
       <c r="G70" s="2"/>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>76</v>
       </c>
@@ -3074,7 +3074,7 @@
       </c>
       <c r="G71" s="2"/>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>76</v>
       </c>
@@ -3095,7 +3095,7 @@
       </c>
       <c r="G72" s="2"/>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>76</v>
       </c>
@@ -3116,7 +3116,7 @@
       </c>
       <c r="G73" s="2"/>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>76</v>
       </c>
@@ -3137,7 +3137,7 @@
       </c>
       <c r="G74" s="2"/>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>76</v>
       </c>
@@ -3158,7 +3158,7 @@
       </c>
       <c r="G75" s="2"/>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>76</v>
       </c>
@@ -3179,7 +3179,7 @@
       </c>
       <c r="G76" s="2"/>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>76</v>
       </c>
@@ -3200,7 +3200,7 @@
       </c>
       <c r="G77" s="2"/>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>76</v>
       </c>
@@ -3221,7 +3221,7 @@
       </c>
       <c r="G78" s="2"/>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>76</v>
       </c>
@@ -3242,7 +3242,7 @@
       </c>
       <c r="G79" s="2"/>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>76</v>
       </c>
@@ -3263,7 +3263,7 @@
       </c>
       <c r="G80" s="2"/>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>76</v>
       </c>
@@ -3284,7 +3284,7 @@
       </c>
       <c r="G81" s="2"/>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>76</v>
       </c>
@@ -3305,7 +3305,7 @@
       </c>
       <c r="G82" s="2"/>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>76</v>
       </c>
@@ -3326,7 +3326,7 @@
       </c>
       <c r="G83" s="2"/>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>76</v>
       </c>
@@ -3347,7 +3347,7 @@
       </c>
       <c r="G84" s="2"/>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>76</v>
       </c>
@@ -3368,7 +3368,7 @@
       </c>
       <c r="G85" s="2"/>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>76</v>
       </c>
@@ -3389,7 +3389,7 @@
       </c>
       <c r="G86" s="2"/>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>76</v>
       </c>
@@ -3410,7 +3410,7 @@
       </c>
       <c r="G87" s="2"/>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>76</v>
       </c>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="G88" s="2"/>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>76</v>
       </c>
@@ -3452,7 +3452,7 @@
       </c>
       <c r="G89" s="2"/>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>76</v>
       </c>
@@ -3473,7 +3473,7 @@
       </c>
       <c r="G90" s="2"/>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>76</v>
       </c>
@@ -3494,7 +3494,7 @@
       </c>
       <c r="G91" s="2"/>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>76</v>
       </c>
@@ -3515,7 +3515,7 @@
       </c>
       <c r="G92" s="2"/>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>76</v>
       </c>
@@ -3536,7 +3536,7 @@
       </c>
       <c r="G93" s="2"/>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>76</v>
       </c>
@@ -3557,7 +3557,7 @@
       </c>
       <c r="G94" s="2"/>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>76</v>
       </c>
@@ -3578,7 +3578,7 @@
       </c>
       <c r="G95" s="2"/>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>76</v>
       </c>
@@ -3599,7 +3599,7 @@
       </c>
       <c r="G96" s="2"/>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>76</v>
       </c>
@@ -3620,7 +3620,7 @@
       </c>
       <c r="G97" s="2"/>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>76</v>
       </c>
@@ -3641,7 +3641,7 @@
       </c>
       <c r="G98" s="2"/>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>76</v>
       </c>
@@ -3662,7 +3662,7 @@
       </c>
       <c r="G99" s="2"/>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>76</v>
       </c>
@@ -3683,7 +3683,7 @@
       </c>
       <c r="G100" s="2"/>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>76</v>
       </c>
@@ -3704,7 +3704,7 @@
       </c>
       <c r="G101" s="2"/>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>76</v>
       </c>
@@ -3725,9 +3725,9 @@
       </c>
       <c r="G102" s="2"/>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B103" t="s">
         <v>64</v>
@@ -3746,49 +3746,49 @@
       </c>
       <c r="G103" s="2"/>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B104" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="C104" t="s">
         <v>170</v>
       </c>
       <c r="D104" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="E104" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="F104">
         <v>2</v>
       </c>
       <c r="G104" s="2"/>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B105" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="C105" t="s">
         <v>171</v>
       </c>
       <c r="D105" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="E105" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="F105">
         <v>3</v>
       </c>
       <c r="G105" s="2"/>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>46</v>
       </c>
@@ -3809,7 +3809,7 @@
       </c>
       <c r="G106" s="2"/>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>46</v>
       </c>
@@ -3830,7 +3830,7 @@
       </c>
       <c r="G107" s="2"/>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>51</v>
       </c>
@@ -3853,7 +3853,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>51</v>
       </c>
@@ -3876,7 +3876,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>51</v>
       </c>
@@ -3896,7 +3896,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>51</v>
       </c>
@@ -3929,15 +3929,15 @@
   <dimension ref="A1:B40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.86328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>192</v>
       </c>
@@ -3945,47 +3945,47 @@
         <v>193</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="B2" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.45">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>268</v>
+        <v>276</v>
       </c>
       <c r="B3" s="2">
         <v>2000</v>
       </c>
     </row>
-    <row r="4" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="B4" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.45">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="B5" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.45">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="B6" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>194</v>
       </c>
@@ -3993,7 +3993,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>196</v>
       </c>
@@ -4001,7 +4001,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>197</v>
       </c>
@@ -4009,55 +4009,55 @@
         <v>195</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>198</v>
       </c>
       <c r="B10" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>199</v>
       </c>
       <c r="B11" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>200</v>
       </c>
       <c r="B12" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>201</v>
       </c>
       <c r="B13" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>202</v>
       </c>
       <c r="B14" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>203</v>
       </c>
       <c r="B15" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>204</v>
       </c>
@@ -4065,7 +4065,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>206</v>
       </c>
@@ -4073,7 +4073,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>208</v>
       </c>
@@ -4081,7 +4081,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>210</v>
       </c>
@@ -4089,7 +4089,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>212</v>
       </c>
@@ -4097,7 +4097,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>214</v>
       </c>
@@ -4105,156 +4105,156 @@
         <v>215</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>277</v>
+      </c>
+      <c r="B22" t="s">
         <v>216</v>
       </c>
-      <c r="B22" t="s">
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>278</v>
+      </c>
+      <c r="B23" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A23" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>279</v>
+      </c>
+      <c r="B24" t="s">
         <v>218</v>
       </c>
-      <c r="B23" t="s">
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>280</v>
+      </c>
+      <c r="B25" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A24" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>220</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B26" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A25" t="s">
+      <c r="B27" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>222</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B28" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>281</v>
+      </c>
+      <c r="B29" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A26" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>282</v>
+      </c>
+      <c r="B30" t="s">
         <v>224</v>
       </c>
-      <c r="B26" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A27" t="s">
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>283</v>
+      </c>
+      <c r="B31" t="s">
         <v>225</v>
       </c>
-      <c r="B27" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A28" t="s">
-        <v>226</v>
-      </c>
-      <c r="B28" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A29" t="s">
-        <v>227</v>
-      </c>
-      <c r="B29" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A30" t="s">
-        <v>229</v>
-      </c>
-      <c r="B30" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A31" t="s">
-        <v>275</v>
-      </c>
-      <c r="B31" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>232</v>
+        <v>284</v>
       </c>
       <c r="B32" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="B33">
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="B34">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="B35" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="B36" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="B37" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="B38" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="B39" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="B40" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rename sheets and variables in metadata sheet
Close #58
</commit_message>
<xml_diff>
--- a/tests/testthat/fixtures/metadata/metadata_BEXLTALL.xlsx
+++ b/tests/testthat/fixtures/metadata/metadata_BEXLTALL.xlsx
@@ -8,37 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johan Ejstrud\Dropbox\repo\pxmake\tests\testthat\fixtures\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74036D84-B5C2-4940-99CB-0AEFBCCE56CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C38CB54-3599-4554-906F-D8F58064A08E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="17265" windowHeight="31800" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17265" yWindow="0" windowWidth="23220" windowHeight="31800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Variables_MD" sheetId="1" r:id="rId1"/>
-    <sheet name="Codelists_2MD" sheetId="2" r:id="rId2"/>
-    <sheet name="General_MD" sheetId="3" r:id="rId3"/>
+    <sheet name="General" sheetId="3" r:id="rId1"/>
+    <sheet name="Variables" sheetId="1" r:id="rId2"/>
+    <sheet name="Codelists" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="282">
   <si>
     <t>position</t>
   </si>
   <si>
-    <t>VarName</t>
-  </si>
-  <si>
-    <t>en_varName</t>
-  </si>
-  <si>
-    <t>da_varName</t>
-  </si>
-  <si>
-    <t>kl_varName</t>
-  </si>
-  <si>
     <t>type</t>
   </si>
   <si>
@@ -198,24 +186,12 @@
     <t>code</t>
   </si>
   <si>
-    <t>en_codeLabel</t>
-  </si>
-  <si>
-    <t>da_codeLabel</t>
-  </si>
-  <si>
-    <t>kl_codeLabel</t>
-  </si>
-  <si>
     <t>sortorder</t>
   </si>
   <si>
     <t>precision</t>
   </si>
   <si>
-    <t>PLACE OF BIRTH</t>
-  </si>
-  <si>
     <t>T</t>
   </si>
   <si>
@@ -252,9 +228,6 @@
     <t>3</t>
   </si>
   <si>
-    <t>AGE</t>
-  </si>
-  <si>
     <t>0</t>
   </si>
   <si>
@@ -546,337 +519,355 @@
     <t>lexis squares</t>
   </si>
   <si>
+    <t>kl a</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>lexis parallelogram</t>
+  </si>
+  <si>
+    <t>lexis b-grupper</t>
+  </si>
+  <si>
+    <t>mx</t>
+  </si>
+  <si>
+    <t>Deathrate</t>
+  </si>
+  <si>
+    <t>Dødskvotient</t>
+  </si>
+  <si>
+    <t>kl Dødskvotient</t>
+  </si>
+  <si>
+    <t>qx</t>
+  </si>
+  <si>
+    <t>Mortalityrate</t>
+  </si>
+  <si>
+    <t>Dødshyppighed</t>
+  </si>
+  <si>
+    <t>kl Dødshyppighed</t>
+  </si>
+  <si>
+    <t>lx</t>
+  </si>
+  <si>
+    <t>Survivors</t>
+  </si>
+  <si>
+    <t>Overlevende</t>
+  </si>
+  <si>
+    <t>kl Overlevende</t>
+  </si>
+  <si>
+    <t>ex</t>
+  </si>
+  <si>
+    <t>keyword</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>CONTACT_en</t>
+  </si>
+  <si>
+    <t>Lars Pedersen, LARP@stat.gl</t>
+  </si>
+  <si>
+    <t>CONTACT_da</t>
+  </si>
+  <si>
+    <t>CONTACT_kl</t>
+  </si>
+  <si>
+    <t>NOTE_da</t>
+  </si>
+  <si>
+    <t>NOTE_en</t>
+  </si>
+  <si>
+    <t>NOTE_kl</t>
+  </si>
+  <si>
+    <t>CONTENTS_da</t>
+  </si>
+  <si>
+    <t>CONTENTS_en</t>
+  </si>
+  <si>
+    <t>CONTENTS_kl</t>
+  </si>
+  <si>
+    <t>UNITS_da</t>
+  </si>
+  <si>
+    <t>kvotienter</t>
+  </si>
+  <si>
+    <t>UNITS_en</t>
+  </si>
+  <si>
+    <t>rates</t>
+  </si>
+  <si>
+    <t>UNITS_kl</t>
+  </si>
+  <si>
+    <t>kl kvotienter</t>
+  </si>
+  <si>
+    <t>SOURCE_da</t>
+  </si>
+  <si>
+    <t>Grønlands Statistik</t>
+  </si>
+  <si>
+    <t>SOURCE_kl</t>
+  </si>
+  <si>
+    <t>Naatsorsueqqissaartarfik</t>
+  </si>
+  <si>
+    <t>SOURCE_en</t>
+  </si>
+  <si>
+    <t>Statistics Greenland</t>
+  </si>
+  <si>
+    <t>BE</t>
+  </si>
+  <si>
+    <t>Befolkning</t>
+  </si>
+  <si>
+    <t>Population</t>
+  </si>
+  <si>
+    <t>Innuttaasut</t>
+  </si>
+  <si>
+    <t>DESCRIPTION_en</t>
+  </si>
+  <si>
+    <t>DESCRIPTION_da</t>
+  </si>
+  <si>
+    <t>DESCRIPTION_kl</t>
+  </si>
+  <si>
+    <t>20190124 09:00</t>
+  </si>
+  <si>
+    <t>Annually</t>
+  </si>
+  <si>
+    <t>20220222 09:00</t>
+  </si>
+  <si>
+    <t>LINK_da</t>
+  </si>
+  <si>
+    <t>www.stat.gl/bed202201/m1</t>
+  </si>
+  <si>
+    <t>LINK_en</t>
+  </si>
+  <si>
+    <t>www.stat.gl/bee202201/m1</t>
+  </si>
+  <si>
+    <t>LINK_kl</t>
+  </si>
+  <si>
+    <t>www.stat.gl/ben202201/m1</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>sex</t>
+  </si>
+  <si>
+    <t>Mænd</t>
+  </si>
+  <si>
+    <t>Kvinder</t>
+  </si>
+  <si>
+    <t>Grønland</t>
+  </si>
+  <si>
+    <t>Angutit</t>
+  </si>
+  <si>
+    <t>Arnat</t>
+  </si>
+  <si>
+    <t>Kalaallit Nunaat</t>
+  </si>
+  <si>
+    <t>q1</t>
+  </si>
+  <si>
+    <t>q2</t>
+  </si>
+  <si>
+    <t>q5</t>
+  </si>
+  <si>
+    <t>noteda</t>
+  </si>
+  <si>
+    <t>noteen</t>
+  </si>
+  <si>
+    <t>kl note</t>
+  </si>
+  <si>
+    <t>NOTEX_da</t>
+  </si>
+  <si>
+    <t>NOTEX_en</t>
+  </si>
+  <si>
+    <t>NOTEX_kl</t>
+  </si>
+  <si>
+    <t>notedax</t>
+  </si>
+  <si>
+    <t>noteenx</t>
+  </si>
+  <si>
+    <t>kl note x</t>
+  </si>
+  <si>
+    <t>Life tables, 1982 - &lt;em&gt;[BEELTALL]&lt;/em&gt;</t>
+  </si>
+  <si>
+    <t>Overlevelsestavler, 1982 - &lt;em&gt;[BEDLTALL]&lt;/em&gt;</t>
+  </si>
+  <si>
+    <t>kl Overlevelsestavler 1982 - &lt;em&gt;[BENLTALL]&lt;/em&gt;</t>
+  </si>
+  <si>
+    <t>kl Overlevelsestavler</t>
+  </si>
+  <si>
+    <t>Life tables</t>
+  </si>
+  <si>
+    <t>Overlevelsestavler</t>
+  </si>
+  <si>
+    <t>CHARSET</t>
+  </si>
+  <si>
+    <t>LANGUAGE</t>
+  </si>
+  <si>
+    <t>en</t>
+  </si>
+  <si>
+    <t>LANGUAGES</t>
+  </si>
+  <si>
+    <t>en","da","kl</t>
+  </si>
+  <si>
+    <t>MATRIX</t>
+  </si>
+  <si>
+    <t>BEXLTALL</t>
+  </si>
+  <si>
+    <t>DECIMALS</t>
+  </si>
+  <si>
+    <t>SHOWDECIMALS</t>
+  </si>
+  <si>
+    <t>calc type</t>
+  </si>
+  <si>
+    <t>no of years</t>
+  </si>
+  <si>
+    <t>antal</t>
+  </si>
+  <si>
+    <t>amerlassusaat</t>
+  </si>
+  <si>
+    <t>FIGURES</t>
+  </si>
+  <si>
+    <t>20230222 09:00</t>
+  </si>
+  <si>
+    <t>ANSI</t>
+  </si>
+  <si>
+    <t>AXIS-VERSION</t>
+  </si>
+  <si>
+    <t>SUBJECT-CODE</t>
+  </si>
+  <si>
+    <t>SUBJECT-AREA_da</t>
+  </si>
+  <si>
+    <t>SUBJECT-AREA_en</t>
+  </si>
+  <si>
+    <t>SUBJECT-AREA_kl</t>
+  </si>
+  <si>
+    <t>CREATION-DATE</t>
+  </si>
+  <si>
+    <t>UPDATE-FREQUENCY</t>
+  </si>
+  <si>
+    <t>LAST-UPDATED</t>
+  </si>
+  <si>
+    <t>NEXT-UPDATE</t>
+  </si>
+  <si>
+    <t>variable</t>
+  </si>
+  <si>
+    <t>en_long_name</t>
+  </si>
+  <si>
+    <t>da_long_name</t>
+  </si>
+  <si>
+    <t>kl_long_name</t>
+  </si>
+  <si>
+    <t>en_code_label</t>
+  </si>
+  <si>
+    <t>da_code_label</t>
+  </si>
+  <si>
+    <t>kl_code_label</t>
+  </si>
+  <si>
     <t>lexis a-grupper</t>
-  </si>
-  <si>
-    <t>kl a</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>lexis parallelogram</t>
-  </si>
-  <si>
-    <t>lexis b-grupper</t>
-  </si>
-  <si>
-    <t>mx</t>
-  </si>
-  <si>
-    <t>Deathrate</t>
-  </si>
-  <si>
-    <t>Dødskvotient</t>
-  </si>
-  <si>
-    <t>kl Dødskvotient</t>
-  </si>
-  <si>
-    <t>qx</t>
-  </si>
-  <si>
-    <t>Mortalityrate</t>
-  </si>
-  <si>
-    <t>Dødshyppighed</t>
-  </si>
-  <si>
-    <t>kl Dødshyppighed</t>
-  </si>
-  <si>
-    <t>lx</t>
-  </si>
-  <si>
-    <t>Survivors</t>
-  </si>
-  <si>
-    <t>Overlevende</t>
-  </si>
-  <si>
-    <t>kl Overlevende</t>
-  </si>
-  <si>
-    <t>ex</t>
-  </si>
-  <si>
-    <t>keyword</t>
-  </si>
-  <si>
-    <t>value</t>
-  </si>
-  <si>
-    <t>CONTACT_en</t>
-  </si>
-  <si>
-    <t>Lars Pedersen, LARP@stat.gl</t>
-  </si>
-  <si>
-    <t>CONTACT_da</t>
-  </si>
-  <si>
-    <t>CONTACT_kl</t>
-  </si>
-  <si>
-    <t>NOTE_da</t>
-  </si>
-  <si>
-    <t>NOTE_en</t>
-  </si>
-  <si>
-    <t>NOTE_kl</t>
-  </si>
-  <si>
-    <t>CONTENTS_da</t>
-  </si>
-  <si>
-    <t>CONTENTS_en</t>
-  </si>
-  <si>
-    <t>CONTENTS_kl</t>
-  </si>
-  <si>
-    <t>UNITS_da</t>
-  </si>
-  <si>
-    <t>kvotienter</t>
-  </si>
-  <si>
-    <t>UNITS_en</t>
-  </si>
-  <si>
-    <t>rates</t>
-  </si>
-  <si>
-    <t>UNITS_kl</t>
-  </si>
-  <si>
-    <t>kl kvotienter</t>
-  </si>
-  <si>
-    <t>SOURCE_da</t>
-  </si>
-  <si>
-    <t>Grønlands Statistik</t>
-  </si>
-  <si>
-    <t>SOURCE_kl</t>
-  </si>
-  <si>
-    <t>Naatsorsueqqissaartarfik</t>
-  </si>
-  <si>
-    <t>SOURCE_en</t>
-  </si>
-  <si>
-    <t>Statistics Greenland</t>
-  </si>
-  <si>
-    <t>BE</t>
-  </si>
-  <si>
-    <t>Befolkning</t>
-  </si>
-  <si>
-    <t>Population</t>
-  </si>
-  <si>
-    <t>Innuttaasut</t>
-  </si>
-  <si>
-    <t>DESCRIPTION_en</t>
-  </si>
-  <si>
-    <t>DESCRIPTION_da</t>
-  </si>
-  <si>
-    <t>DESCRIPTION_kl</t>
-  </si>
-  <si>
-    <t>20190124 09:00</t>
-  </si>
-  <si>
-    <t>Annually</t>
-  </si>
-  <si>
-    <t>20220222 09:00</t>
-  </si>
-  <si>
-    <t>LINK_da</t>
-  </si>
-  <si>
-    <t>www.stat.gl/bed202201/m1</t>
-  </si>
-  <si>
-    <t>LINK_en</t>
-  </si>
-  <si>
-    <t>www.stat.gl/bee202201/m1</t>
-  </si>
-  <si>
-    <t>LINK_kl</t>
-  </si>
-  <si>
-    <t>www.stat.gl/ben202201/m1</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>SEX</t>
-  </si>
-  <si>
-    <t>sex</t>
-  </si>
-  <si>
-    <t>Mænd</t>
-  </si>
-  <si>
-    <t>Kvinder</t>
-  </si>
-  <si>
-    <t>Grønland</t>
-  </si>
-  <si>
-    <t>Angutit</t>
-  </si>
-  <si>
-    <t>Arnat</t>
-  </si>
-  <si>
-    <t>Kalaallit Nunaat</t>
-  </si>
-  <si>
-    <t>q1</t>
-  </si>
-  <si>
-    <t>q2</t>
-  </si>
-  <si>
-    <t>q5</t>
-  </si>
-  <si>
-    <t>noteda</t>
-  </si>
-  <si>
-    <t>noteen</t>
-  </si>
-  <si>
-    <t>kl note</t>
-  </si>
-  <si>
-    <t>NOTEX_da</t>
-  </si>
-  <si>
-    <t>NOTEX_en</t>
-  </si>
-  <si>
-    <t>NOTEX_kl</t>
-  </si>
-  <si>
-    <t>notedax</t>
-  </si>
-  <si>
-    <t>noteenx</t>
-  </si>
-  <si>
-    <t>kl note x</t>
-  </si>
-  <si>
-    <t>Life tables, 1982 - &lt;em&gt;[BEELTALL]&lt;/em&gt;</t>
-  </si>
-  <si>
-    <t>Overlevelsestavler, 1982 - &lt;em&gt;[BEDLTALL]&lt;/em&gt;</t>
-  </si>
-  <si>
-    <t>kl Overlevelsestavler 1982 - &lt;em&gt;[BENLTALL]&lt;/em&gt;</t>
-  </si>
-  <si>
-    <t>kl Overlevelsestavler</t>
-  </si>
-  <si>
-    <t>Life tables</t>
-  </si>
-  <si>
-    <t>Overlevelsestavler</t>
-  </si>
-  <si>
-    <t>CHARSET</t>
-  </si>
-  <si>
-    <t>LANGUAGE</t>
-  </si>
-  <si>
-    <t>en</t>
-  </si>
-  <si>
-    <t>LANGUAGES</t>
-  </si>
-  <si>
-    <t>en","da","kl</t>
-  </si>
-  <si>
-    <t>MATRIX</t>
-  </si>
-  <si>
-    <t>BEXLTALL</t>
-  </si>
-  <si>
-    <t>DECIMALS</t>
-  </si>
-  <si>
-    <t>SHOWDECIMALS</t>
-  </si>
-  <si>
-    <t>calc type</t>
-  </si>
-  <si>
-    <t>no of years</t>
-  </si>
-  <si>
-    <t>antal</t>
-  </si>
-  <si>
-    <t>amerlassusaat</t>
-  </si>
-  <si>
-    <t>FIGURES</t>
-  </si>
-  <si>
-    <t>20230222 09:00</t>
-  </si>
-  <si>
-    <t>ANSI</t>
-  </si>
-  <si>
-    <t>AXIS-VERSION</t>
-  </si>
-  <si>
-    <t>SUBJECT-CODE</t>
-  </si>
-  <si>
-    <t>SUBJECT-AREA_da</t>
-  </si>
-  <si>
-    <t>SUBJECT-AREA_en</t>
-  </si>
-  <si>
-    <t>SUBJECT-AREA_kl</t>
-  </si>
-  <si>
-    <t>CREATION-DATE</t>
-  </si>
-  <si>
-    <t>UPDATE-FREQUENCY</t>
-  </si>
-  <si>
-    <t>LAST-UPDATED</t>
-  </si>
-  <si>
-    <t>NEXT-UPDATE</t>
   </si>
 </sst>
 </file>
@@ -920,14 +911,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1266,24 +1260,364 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:B40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>249</v>
+      </c>
+      <c r="B2" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>265</v>
+      </c>
+      <c r="B3" s="2">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>250</v>
+      </c>
+      <c r="B4" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>252</v>
+      </c>
+      <c r="B5" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>254</v>
+      </c>
+      <c r="B6" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>184</v>
+      </c>
+      <c r="B7" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>186</v>
+      </c>
+      <c r="B8" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>187</v>
+      </c>
+      <c r="B9" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>188</v>
+      </c>
+      <c r="B10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>189</v>
+      </c>
+      <c r="B11" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>190</v>
+      </c>
+      <c r="B12" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>191</v>
+      </c>
+      <c r="B13" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>192</v>
+      </c>
+      <c r="B14" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>193</v>
+      </c>
+      <c r="B15" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>194</v>
+      </c>
+      <c r="B16" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>196</v>
+      </c>
+      <c r="B17" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>198</v>
+      </c>
+      <c r="B18" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>200</v>
+      </c>
+      <c r="B19" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>202</v>
+      </c>
+      <c r="B20" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>204</v>
+      </c>
+      <c r="B21" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>266</v>
+      </c>
+      <c r="B22" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>267</v>
+      </c>
+      <c r="B23" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>268</v>
+      </c>
+      <c r="B24" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>269</v>
+      </c>
+      <c r="B25" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>210</v>
+      </c>
+      <c r="B26" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>211</v>
+      </c>
+      <c r="B27" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>212</v>
+      </c>
+      <c r="B28" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>270</v>
+      </c>
+      <c r="B29" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>271</v>
+      </c>
+      <c r="B30" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>272</v>
+      </c>
+      <c r="B31" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>273</v>
+      </c>
+      <c r="B32" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>256</v>
+      </c>
+      <c r="B33">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>257</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>216</v>
+      </c>
+      <c r="B35" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>218</v>
+      </c>
+      <c r="B36" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>220</v>
+      </c>
+      <c r="B37" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>237</v>
+      </c>
+      <c r="B38" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>238</v>
+      </c>
+      <c r="B39" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>239</v>
+      </c>
+      <c r="B40" t="s">
+        <v>242</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F70" sqref="F70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
@@ -1291,271 +1625,271 @@
     <col min="15" max="15" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="J1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="K1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="L1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="M1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="N1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="O1" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" t="s">
         <v>20</v>
       </c>
-      <c r="C3" t="s">
+      <c r="K3" t="s">
         <v>20</v>
       </c>
-      <c r="D3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="L3" t="s">
         <v>22</v>
-      </c>
-      <c r="F3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" t="s">
-        <v>24</v>
-      </c>
-      <c r="K3" t="s">
-        <v>24</v>
-      </c>
-      <c r="L3" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>259</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" t="s">
         <v>27</v>
       </c>
-      <c r="B4" t="s">
+      <c r="K4" t="s">
         <v>28</v>
       </c>
-      <c r="C4" t="s">
-        <v>270</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="L4" t="s">
         <v>29</v>
-      </c>
-      <c r="E4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J4" t="s">
-        <v>31</v>
-      </c>
-      <c r="K4" t="s">
-        <v>32</v>
-      </c>
-      <c r="L4" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K5" t="s">
+        <v>34</v>
+      </c>
+      <c r="L5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M5" t="s">
         <v>35</v>
       </c>
-      <c r="C5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="N5" t="s">
         <v>36</v>
       </c>
-      <c r="E5" t="s">
+      <c r="O5" t="s">
         <v>37</v>
-      </c>
-      <c r="F5" t="s">
-        <v>23</v>
-      </c>
-      <c r="J5" t="s">
-        <v>38</v>
-      </c>
-      <c r="K5" t="s">
-        <v>38</v>
-      </c>
-      <c r="L5" t="s">
-        <v>38</v>
-      </c>
-      <c r="M5" t="s">
-        <v>39</v>
-      </c>
-      <c r="N5" t="s">
-        <v>40</v>
-      </c>
-      <c r="O5" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="C6" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="D6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="J6" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="K6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="L6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" t="s">
+        <v>258</v>
+      </c>
+      <c r="D7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" t="s">
         <v>19</v>
       </c>
-      <c r="B7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C7" t="s">
-        <v>269</v>
-      </c>
-      <c r="D7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F7" t="s">
-        <v>23</v>
-      </c>
       <c r="J7" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="K7" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="L7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J8" t="s">
         <v>50</v>
       </c>
-      <c r="B8" t="s">
+      <c r="K8" t="s">
         <v>51</v>
       </c>
-      <c r="C8" t="s">
-        <v>51</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="L8" t="s">
         <v>52</v>
-      </c>
-      <c r="E8" t="s">
-        <v>53</v>
-      </c>
-      <c r="F8" t="s">
-        <v>23</v>
-      </c>
-      <c r="J8" t="s">
-        <v>54</v>
-      </c>
-      <c r="K8" t="s">
-        <v>55</v>
-      </c>
-      <c r="L8" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="C9" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="D9" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="E9" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
       <c r="F9" t="s">
-        <v>273</v>
+        <v>262</v>
       </c>
     </row>
   </sheetData>
@@ -1563,12 +1897,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G111"/>
   <sheetViews>
-    <sheetView topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="D90" sqref="D90"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D107" sqref="D107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1576,49 +1910,49 @@
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>62</v>
+    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -1627,19 +1961,19 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C3" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D3" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="E3" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="F3">
         <v>2</v>
@@ -1648,19 +1982,19 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
       <c r="C4" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="D4" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="E4" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -1669,19 +2003,19 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
       <c r="C5" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="D5" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E5" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="F5">
         <v>2</v>
@@ -1690,19 +2024,19 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
+        <v>233</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s">
         <v>28</v>
       </c>
-      <c r="B6" t="s">
-        <v>244</v>
-      </c>
-      <c r="C6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" t="s">
-        <v>32</v>
-      </c>
       <c r="E6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F6">
         <v>3</v>
@@ -1711,19 +2045,19 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B7" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="C7" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="D7" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="E7" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -1732,19 +2066,19 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="C8" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="D8" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="E8" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -1753,19 +2087,19 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C9" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="D9" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="E9" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="F9">
         <v>2</v>
@@ -1774,19 +2108,19 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B10" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C10" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="D10" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="E10" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="F10">
         <v>3</v>
@@ -1795,19 +2129,19 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="C11" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="D11" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="E11" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="F11">
         <v>4</v>
@@ -1816,19 +2150,19 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="C12" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="D12" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="E12" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="F12">
         <v>5</v>
@@ -1837,19 +2171,19 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B13" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="C13" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="D13" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="E13" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="F13">
         <v>6</v>
@@ -1858,19 +2192,19 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B14" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C14" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="D14" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="E14" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F14">
         <v>7</v>
@@ -1879,19 +2213,19 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="C15" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D15" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="E15" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="F15">
         <v>8</v>
@@ -1900,19 +2234,19 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B16" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C16" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="D16" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="E16" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="F16">
         <v>9</v>
@@ -1921,19 +2255,19 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B17" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="C17" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="D17" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="E17" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="F17">
         <v>10</v>
@@ -1942,19 +2276,19 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" t="s">
         <v>76</v>
       </c>
-      <c r="B18" t="s">
-        <v>85</v>
-      </c>
       <c r="C18" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="D18" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E18" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="F18">
         <v>11</v>
@@ -1963,19 +2297,19 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B19" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="C19" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="D19" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="E19" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="F19">
         <v>12</v>
@@ -1984,19 +2318,19 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B20" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="C20" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="D20" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="E20" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="F20">
         <v>13</v>
@@ -2005,19 +2339,19 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B21" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="C21" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="D21" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="E21" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="F21">
         <v>14</v>
@@ -2026,19 +2360,19 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B22" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="C22" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="D22" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="E22" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="F22">
         <v>15</v>
@@ -2047,19 +2381,19 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B23" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C23" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="D23" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="E23" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="F23">
         <v>16</v>
@@ -2068,19 +2402,19 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B24" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="C24" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="D24" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="E24" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="F24">
         <v>17</v>
@@ -2089,19 +2423,19 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B25" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="C25" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="D25" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="E25" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="F25">
         <v>18</v>
@@ -2110,19 +2444,19 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B26" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="C26" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="D26" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="E26" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="F26">
         <v>19</v>
@@ -2131,19 +2465,19 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B27" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="C27" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="D27" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="E27" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="F27">
         <v>20</v>
@@ -2152,19 +2486,19 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B28" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="C28" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="D28" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="E28" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="F28">
         <v>21</v>
@@ -2173,19 +2507,19 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B29" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="C29" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="D29" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E29" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="F29">
         <v>22</v>
@@ -2194,19 +2528,19 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="C30" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="D30" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="E30" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="F30">
         <v>23</v>
@@ -2215,19 +2549,19 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="C31" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="D31" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="E31" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="F31">
         <v>24</v>
@@ -2236,19 +2570,19 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="C32" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="D32" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="E32" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="F32">
         <v>25</v>
@@ -2257,19 +2591,19 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="C33" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="D33" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="E33" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="F33">
         <v>26</v>
@@ -2278,19 +2612,19 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B34" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="C34" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="D34" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="E34" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="F34">
         <v>27</v>
@@ -2299,19 +2633,19 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B35" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C35" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="D35" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="E35" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="F35">
         <v>28</v>
@@ -2320,19 +2654,19 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B36" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="C36" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="D36" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="E36" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="F36">
         <v>29</v>
@@ -2341,19 +2675,19 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B37" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="C37" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="D37" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="E37" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="F37">
         <v>30</v>
@@ -2362,19 +2696,19 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B38" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="C38" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="D38" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="E38" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="F38">
         <v>31</v>
@@ -2383,19 +2717,19 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B39" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="C39" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="D39" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="E39" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="F39">
         <v>32</v>
@@ -2404,19 +2738,19 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B40" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="C40" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="D40" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="E40" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="F40">
         <v>33</v>
@@ -2425,19 +2759,19 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B41" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="C41" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="D41" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="E41" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="F41">
         <v>34</v>
@@ -2446,19 +2780,19 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B42" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="C42" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="D42" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="E42" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="F42">
         <v>35</v>
@@ -2467,19 +2801,19 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B43" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C43" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="D43" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="E43" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="F43">
         <v>36</v>
@@ -2488,19 +2822,19 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B44" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="C44" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="D44" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="E44" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="F44">
         <v>37</v>
@@ -2509,19 +2843,19 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B45" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="C45" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D45" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="E45" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="F45">
         <v>38</v>
@@ -2530,19 +2864,19 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B46" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="C46" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="D46" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="E46" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="F46">
         <v>39</v>
@@ -2551,19 +2885,19 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B47" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="C47" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="D47" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="E47" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="F47">
         <v>40</v>
@@ -2572,19 +2906,19 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B48" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="C48" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="D48" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="E48" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="F48">
         <v>41</v>
@@ -2593,19 +2927,19 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B49" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="C49" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="D49" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="E49" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="F49">
         <v>42</v>
@@ -2614,19 +2948,19 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B50" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="C50" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="D50" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="E50" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="F50">
         <v>43</v>
@@ -2635,19 +2969,19 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B51" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="C51" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="D51" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="E51" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="F51">
         <v>44</v>
@@ -2656,19 +2990,19 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B52" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="C52" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="D52" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="E52" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="F52">
         <v>45</v>
@@ -2677,19 +3011,19 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B53" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="C53" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="D53" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="E53" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="F53">
         <v>46</v>
@@ -2698,19 +3032,19 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B54" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="C54" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="D54" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="E54" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="F54">
         <v>47</v>
@@ -2719,19 +3053,19 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B55" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="C55" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="D55" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="E55" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="F55">
         <v>48</v>
@@ -2740,19 +3074,19 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B56" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="C56" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="D56" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="E56" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="F56">
         <v>49</v>
@@ -2761,19 +3095,19 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B57" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="C57" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="D57" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="E57" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="F57">
         <v>50</v>
@@ -2782,19 +3116,19 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B58" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="C58" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="D58" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="E58" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="F58">
         <v>51</v>
@@ -2803,19 +3137,19 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B59" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="C59" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="D59" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="E59" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="F59">
         <v>52</v>
@@ -2824,19 +3158,19 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B60" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="C60" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="D60" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="E60" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="F60">
         <v>53</v>
@@ -2845,19 +3179,19 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B61" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="C61" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="D61" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="E61" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="F61">
         <v>54</v>
@@ -2866,19 +3200,19 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B62" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="C62" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="D62" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="E62" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="F62">
         <v>55</v>
@@ -2887,19 +3221,19 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B63" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="C63" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="D63" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="E63" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="F63">
         <v>56</v>
@@ -2908,19 +3242,19 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B64" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="C64" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="D64" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="E64" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="F64">
         <v>57</v>
@@ -2929,19 +3263,19 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B65" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="C65" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="D65" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="E65" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="F65">
         <v>58</v>
@@ -2950,19 +3284,19 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B66" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="C66" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="D66" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="E66" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="F66">
         <v>59</v>
@@ -2971,19 +3305,19 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B67" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="C67" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="D67" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="E67" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="F67">
         <v>60</v>
@@ -2992,19 +3326,19 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B68" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="C68" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="D68" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="E68" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="F68">
         <v>61</v>
@@ -3013,19 +3347,19 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B69" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="C69" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="D69" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="E69" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="F69">
         <v>62</v>
@@ -3034,19 +3368,19 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B70" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="C70" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="D70" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E70" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="F70">
         <v>63</v>
@@ -3055,19 +3389,19 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B71" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="C71" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="D71" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="E71" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="F71">
         <v>64</v>
@@ -3076,19 +3410,19 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B72" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="C72" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="D72" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="E72" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="F72">
         <v>65</v>
@@ -3097,19 +3431,19 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B73" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="C73" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="D73" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="E73" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="F73">
         <v>66</v>
@@ -3118,19 +3452,19 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B74" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="C74" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="D74" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="E74" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="F74">
         <v>67</v>
@@ -3139,19 +3473,19 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B75" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="C75" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="D75" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="E75" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="F75">
         <v>68</v>
@@ -3160,19 +3494,19 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B76" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="C76" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="D76" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="E76" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="F76">
         <v>69</v>
@@ -3181,19 +3515,19 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B77" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="C77" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="D77" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="E77" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="F77">
         <v>70</v>
@@ -3202,19 +3536,19 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B78" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C78" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="D78" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="E78" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="F78">
         <v>71</v>
@@ -3223,19 +3557,19 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B79" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="C79" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="D79" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="E79" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="F79">
         <v>72</v>
@@ -3244,19 +3578,19 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B80" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="C80" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="D80" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="E80" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="F80">
         <v>73</v>
@@ -3265,19 +3599,19 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B81" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="C81" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="D81" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="E81" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="F81">
         <v>74</v>
@@ -3286,19 +3620,19 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B82" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="C82" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="D82" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="E82" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="F82">
         <v>75</v>
@@ -3307,19 +3641,19 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B83" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="C83" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="D83" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="E83" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="F83">
         <v>76</v>
@@ -3328,19 +3662,19 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B84" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="C84" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="D84" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="E84" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="F84">
         <v>77</v>
@@ -3349,19 +3683,19 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B85" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="C85" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="D85" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="E85" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="F85">
         <v>78</v>
@@ -3370,19 +3704,19 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B86" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="C86" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="D86" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="E86" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="F86">
         <v>79</v>
@@ -3391,19 +3725,19 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B87" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="C87" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="D87" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="E87" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="F87">
         <v>80</v>
@@ -3412,19 +3746,19 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B88" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="C88" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D88" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="E88" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="F88">
         <v>81</v>
@@ -3433,19 +3767,19 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B89" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="C89" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="D89" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="E89" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="F89">
         <v>82</v>
@@ -3454,19 +3788,19 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B90" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="C90" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="D90" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="E90" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="F90">
         <v>83</v>
@@ -3475,19 +3809,19 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B91" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="C91" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="D91" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="E91" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="F91">
         <v>84</v>
@@ -3496,19 +3830,19 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B92" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="C92" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="D92" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="E92" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="F92">
         <v>85</v>
@@ -3517,19 +3851,19 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B93" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="C93" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="D93" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="E93" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="F93">
         <v>86</v>
@@ -3538,19 +3872,19 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B94" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="C94" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="D94" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="E94" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="F94">
         <v>87</v>
@@ -3559,19 +3893,19 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B95" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="C95" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="D95" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="E95" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="F95">
         <v>88</v>
@@ -3580,19 +3914,19 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B96" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="C96" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="D96" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="E96" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="F96">
         <v>89</v>
@@ -3601,19 +3935,19 @@
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B97" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C97" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="D97" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="E97" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="F97">
         <v>90</v>
@@ -3622,19 +3956,19 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B98" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="C98" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="D98" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="E98" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="F98">
         <v>91</v>
@@ -3643,19 +3977,19 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B99" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="C99" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="D99" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="E99" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="F99">
         <v>92</v>
@@ -3664,19 +3998,19 @@
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B100" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="C100" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="D100" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="E100" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="F100">
         <v>93</v>
@@ -3685,19 +4019,19 @@
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B101" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="C101" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="D101" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="E101" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="F101">
         <v>94</v>
@@ -3706,19 +4040,19 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B102" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="C102" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="D102" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="E102" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="F102">
         <v>95</v>
@@ -3727,19 +4061,19 @@
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="B103" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C103" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D103" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E103" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F103">
         <v>1</v>
@@ -3748,19 +4082,19 @@
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="B104" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="C104" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="D104" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
       <c r="E104" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
       <c r="F104">
         <v>2</v>
@@ -3769,19 +4103,19 @@
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="B105" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="C105" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="D105" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
       <c r="E105" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
       <c r="F105">
         <v>3</v>
@@ -3790,19 +4124,19 @@
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B106" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C106" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="D106" t="s">
-        <v>174</v>
+        <v>281</v>
       </c>
       <c r="E106" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="F106">
         <v>1</v>
@@ -3811,19 +4145,19 @@
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B107" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="C107" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="D107" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="E107" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F107">
         <v>2</v>
@@ -3832,65 +4166,65 @@
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B108" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="C108" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="D108" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="E108" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="F108">
         <v>1</v>
       </c>
       <c r="G108" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B109" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="C109" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="D109" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="E109" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="F109">
         <v>2</v>
       </c>
       <c r="G109" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B110" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C110" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="D110" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="E110" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="F110">
         <v>3</v>
@@ -3898,363 +4232,25 @@
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
+        <v>47</v>
+      </c>
+      <c r="B111" t="s">
+        <v>181</v>
+      </c>
+      <c r="C111" t="s">
+        <v>50</v>
+      </c>
+      <c r="D111" t="s">
         <v>51</v>
       </c>
-      <c r="B111" t="s">
-        <v>191</v>
-      </c>
-      <c r="C111" t="s">
-        <v>54</v>
-      </c>
-      <c r="D111" t="s">
-        <v>55</v>
-      </c>
       <c r="E111" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="F111">
         <v>4</v>
       </c>
       <c r="G111" t="s">
-        <v>70</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B40"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>260</v>
-      </c>
-      <c r="B2" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>276</v>
-      </c>
-      <c r="B3" s="2">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>261</v>
-      </c>
-      <c r="B4" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>263</v>
-      </c>
-      <c r="B5" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>265</v>
-      </c>
-      <c r="B6" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>194</v>
-      </c>
-      <c r="B7" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>196</v>
-      </c>
-      <c r="B8" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>197</v>
-      </c>
-      <c r="B9" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>198</v>
-      </c>
-      <c r="B10" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>199</v>
-      </c>
-      <c r="B11" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>200</v>
-      </c>
-      <c r="B12" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>201</v>
-      </c>
-      <c r="B13" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>202</v>
-      </c>
-      <c r="B14" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>203</v>
-      </c>
-      <c r="B15" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>204</v>
-      </c>
-      <c r="B16" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>206</v>
-      </c>
-      <c r="B17" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>208</v>
-      </c>
-      <c r="B18" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>210</v>
-      </c>
-      <c r="B19" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>212</v>
-      </c>
-      <c r="B20" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>214</v>
-      </c>
-      <c r="B21" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>277</v>
-      </c>
-      <c r="B22" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>278</v>
-      </c>
-      <c r="B23" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>279</v>
-      </c>
-      <c r="B24" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>280</v>
-      </c>
-      <c r="B25" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>220</v>
-      </c>
-      <c r="B26" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>221</v>
-      </c>
-      <c r="B27" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>222</v>
-      </c>
-      <c r="B28" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>281</v>
-      </c>
-      <c r="B29" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>282</v>
-      </c>
-      <c r="B30" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>283</v>
-      </c>
-      <c r="B31" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>284</v>
-      </c>
-      <c r="B32" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>267</v>
-      </c>
-      <c r="B33">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>268</v>
-      </c>
-      <c r="B34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>226</v>
-      </c>
-      <c r="B35" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>228</v>
-      </c>
-      <c r="B36" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>230</v>
-      </c>
-      <c r="B37" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>248</v>
-      </c>
-      <c r="B38" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>249</v>
-      </c>
-      <c r="B39" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>250</v>
-      </c>
-      <c r="B40" t="s">
-        <v>253</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bugfix: complete data by using values both from codelist and data
Close #79
</commit_message>
<xml_diff>
--- a/tests/testthat/fixtures/metadata/metadata_BEXLTALL.xlsx
+++ b/tests/testthat/fixtures/metadata/metadata_BEXLTALL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johan Ejstrud\Dropbox\repo\pxmake\tests\testthat\fixtures\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C38CB54-3599-4554-906F-D8F58064A08E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BBC8C6C-AAD8-4053-87C6-D44ED4321E77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17265" yWindow="0" windowWidth="23220" windowHeight="31800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16680" yWindow="0" windowWidth="24210" windowHeight="31680" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="282">
   <si>
     <t>position</t>
   </si>
@@ -1602,7 +1602,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F70" sqref="F70"/>
     </sheetView>
   </sheetViews>
@@ -1899,10 +1899,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G111"/>
+  <dimension ref="A1:G112"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D107" sqref="D107"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="G103" sqref="G103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4061,22 +4061,22 @@
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>224</v>
-      </c>
-      <c r="B103" t="s">
-        <v>56</v>
-      </c>
-      <c r="C103" t="s">
-        <v>20</v>
-      </c>
-      <c r="D103" t="s">
-        <v>21</v>
-      </c>
-      <c r="E103" t="s">
-        <v>22</v>
+        <v>31</v>
+      </c>
+      <c r="B103">
+        <v>99</v>
+      </c>
+      <c r="C103">
+        <v>99</v>
+      </c>
+      <c r="D103">
+        <v>99</v>
+      </c>
+      <c r="E103">
+        <v>99</v>
       </c>
       <c r="F103">
-        <v>1</v>
+        <v>99</v>
       </c>
       <c r="G103" s="2"/>
     </row>
@@ -4085,19 +4085,19 @@
         <v>224</v>
       </c>
       <c r="B104" t="s">
-        <v>222</v>
+        <v>56</v>
       </c>
       <c r="C104" t="s">
-        <v>161</v>
+        <v>20</v>
       </c>
       <c r="D104" t="s">
-        <v>225</v>
+        <v>21</v>
       </c>
       <c r="E104" t="s">
-        <v>228</v>
+        <v>22</v>
       </c>
       <c r="F104">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G104" s="2"/>
     </row>
@@ -4106,40 +4106,40 @@
         <v>224</v>
       </c>
       <c r="B105" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C105" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D105" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E105" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F105">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G105" s="2"/>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>42</v>
+        <v>224</v>
       </c>
       <c r="B106" t="s">
-        <v>163</v>
+        <v>223</v>
       </c>
       <c r="C106" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D106" t="s">
-        <v>281</v>
+        <v>226</v>
       </c>
       <c r="E106" t="s">
-        <v>165</v>
+        <v>229</v>
       </c>
       <c r="F106">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G106" s="2"/>
     </row>
@@ -4148,63 +4148,61 @@
         <v>42</v>
       </c>
       <c r="B107" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C107" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D107" t="s">
-        <v>168</v>
+        <v>281</v>
       </c>
       <c r="E107" t="s">
-        <v>45</v>
+        <v>165</v>
       </c>
       <c r="F107">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G107" s="2"/>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B108" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C108" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D108" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="E108" t="s">
-        <v>172</v>
+        <v>45</v>
       </c>
       <c r="F108">
-        <v>1</v>
-      </c>
-      <c r="G108" t="s">
-        <v>69</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="G108" s="2"/>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>47</v>
       </c>
       <c r="B109" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C109" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D109" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="E109" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="F109">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G109" t="s">
         <v>69</v>
@@ -4215,19 +4213,22 @@
         <v>47</v>
       </c>
       <c r="B110" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C110" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="D110" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E110" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="F110">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="G110" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
@@ -4235,21 +4236,41 @@
         <v>47</v>
       </c>
       <c r="B111" t="s">
+        <v>177</v>
+      </c>
+      <c r="C111" t="s">
+        <v>178</v>
+      </c>
+      <c r="D111" t="s">
+        <v>179</v>
+      </c>
+      <c r="E111" t="s">
+        <v>180</v>
+      </c>
+      <c r="F111">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>47</v>
+      </c>
+      <c r="B112" t="s">
         <v>181</v>
       </c>
-      <c r="C111" t="s">
+      <c r="C112" t="s">
         <v>50</v>
       </c>
-      <c r="D111" t="s">
+      <c r="D112" t="s">
         <v>51</v>
       </c>
-      <c r="E111" t="s">
+      <c r="E112" t="s">
         <v>52</v>
       </c>
-      <c r="F111">
+      <c r="F112">
         <v>4</v>
       </c>
-      <c r="G111" t="s">
+      <c r="G112" t="s">
         <v>62</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Bugfix: complete data by using values both from codelist and data (#80)
Close #79
</commit_message>
<xml_diff>
--- a/tests/testthat/fixtures/metadata/metadata_BEXLTALL.xlsx
+++ b/tests/testthat/fixtures/metadata/metadata_BEXLTALL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johan Ejstrud\Dropbox\repo\pxmake\tests\testthat\fixtures\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C38CB54-3599-4554-906F-D8F58064A08E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BBC8C6C-AAD8-4053-87C6-D44ED4321E77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17265" yWindow="0" windowWidth="23220" windowHeight="31800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16680" yWindow="0" windowWidth="24210" windowHeight="31680" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="282">
   <si>
     <t>position</t>
   </si>
@@ -1602,7 +1602,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F70" sqref="F70"/>
     </sheetView>
   </sheetViews>
@@ -1899,10 +1899,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G111"/>
+  <dimension ref="A1:G112"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D107" sqref="D107"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="G103" sqref="G103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4061,22 +4061,22 @@
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>224</v>
-      </c>
-      <c r="B103" t="s">
-        <v>56</v>
-      </c>
-      <c r="C103" t="s">
-        <v>20</v>
-      </c>
-      <c r="D103" t="s">
-        <v>21</v>
-      </c>
-      <c r="E103" t="s">
-        <v>22</v>
+        <v>31</v>
+      </c>
+      <c r="B103">
+        <v>99</v>
+      </c>
+      <c r="C103">
+        <v>99</v>
+      </c>
+      <c r="D103">
+        <v>99</v>
+      </c>
+      <c r="E103">
+        <v>99</v>
       </c>
       <c r="F103">
-        <v>1</v>
+        <v>99</v>
       </c>
       <c r="G103" s="2"/>
     </row>
@@ -4085,19 +4085,19 @@
         <v>224</v>
       </c>
       <c r="B104" t="s">
-        <v>222</v>
+        <v>56</v>
       </c>
       <c r="C104" t="s">
-        <v>161</v>
+        <v>20</v>
       </c>
       <c r="D104" t="s">
-        <v>225</v>
+        <v>21</v>
       </c>
       <c r="E104" t="s">
-        <v>228</v>
+        <v>22</v>
       </c>
       <c r="F104">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G104" s="2"/>
     </row>
@@ -4106,40 +4106,40 @@
         <v>224</v>
       </c>
       <c r="B105" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C105" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D105" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E105" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F105">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G105" s="2"/>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>42</v>
+        <v>224</v>
       </c>
       <c r="B106" t="s">
-        <v>163</v>
+        <v>223</v>
       </c>
       <c r="C106" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D106" t="s">
-        <v>281</v>
+        <v>226</v>
       </c>
       <c r="E106" t="s">
-        <v>165</v>
+        <v>229</v>
       </c>
       <c r="F106">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G106" s="2"/>
     </row>
@@ -4148,63 +4148,61 @@
         <v>42</v>
       </c>
       <c r="B107" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C107" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D107" t="s">
-        <v>168</v>
+        <v>281</v>
       </c>
       <c r="E107" t="s">
-        <v>45</v>
+        <v>165</v>
       </c>
       <c r="F107">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G107" s="2"/>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B108" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C108" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D108" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="E108" t="s">
-        <v>172</v>
+        <v>45</v>
       </c>
       <c r="F108">
-        <v>1</v>
-      </c>
-      <c r="G108" t="s">
-        <v>69</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="G108" s="2"/>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>47</v>
       </c>
       <c r="B109" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C109" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D109" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="E109" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="F109">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G109" t="s">
         <v>69</v>
@@ -4215,19 +4213,22 @@
         <v>47</v>
       </c>
       <c r="B110" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C110" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="D110" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E110" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="F110">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="G110" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
@@ -4235,21 +4236,41 @@
         <v>47</v>
       </c>
       <c r="B111" t="s">
+        <v>177</v>
+      </c>
+      <c r="C111" t="s">
+        <v>178</v>
+      </c>
+      <c r="D111" t="s">
+        <v>179</v>
+      </c>
+      <c r="E111" t="s">
+        <v>180</v>
+      </c>
+      <c r="F111">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>47</v>
+      </c>
+      <c r="B112" t="s">
         <v>181</v>
       </c>
-      <c r="C111" t="s">
+      <c r="C112" t="s">
         <v>50</v>
       </c>
-      <c r="D111" t="s">
+      <c r="D112" t="s">
         <v>51</v>
       </c>
-      <c r="E111" t="s">
+      <c r="E112" t="s">
         <v>52</v>
       </c>
-      <c r="F111">
+      <c r="F112">
         <v>4</v>
       </c>
-      <c r="G111" t="s">
+      <c r="G112" t="s">
         <v>62</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Rename metadata sheet 'General' to 'Table'
Close #85
</commit_message>
<xml_diff>
--- a/tests/testthat/fixtures/metadata/metadata_BEXLTALL.xlsx
+++ b/tests/testthat/fixtures/metadata/metadata_BEXLTALL.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johan Ejstrud\Dropbox\repo\pxmake\tests\testthat\fixtures\metadata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johan Ejstrud\My Drive\new\repo\pxmake\tests\testthat\fixtures\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BBC8C6C-AAD8-4053-87C6-D44ED4321E77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59648784-3184-455B-9D97-2AAD1C7D0B99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16680" yWindow="0" windowWidth="24210" windowHeight="31680" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16680" yWindow="0" windowWidth="24210" windowHeight="31680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="General" sheetId="3" r:id="rId1"/>
+    <sheet name="Table" sheetId="3" r:id="rId1"/>
     <sheet name="Variables" sheetId="1" r:id="rId2"/>
     <sheet name="Codelists" sheetId="2" r:id="rId3"/>
   </sheets>
@@ -1263,7 +1263,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
@@ -1901,7 +1901,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="G103" sqref="G103"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Remove need for akward quoting when having multiple langauges
Close #11
</commit_message>
<xml_diff>
--- a/tests/testthat/fixtures/metadata/metadata_BEXLTALL.xlsx
+++ b/tests/testthat/fixtures/metadata/metadata_BEXLTALL.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johan Ejstrud\My Drive\new\repo\pxmake\tests\testthat\fixtures\metadata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johan Ejstrud\Dropbox\repo\pxmake\tests\testthat\fixtures\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59648784-3184-455B-9D97-2AAD1C7D0B99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3418099B-B322-4E4B-AA4E-4F1E4AAD66ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16680" yWindow="0" windowWidth="24210" windowHeight="31680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31680" yWindow="10050" windowWidth="24210" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="3" r:id="rId1"/>
@@ -783,9 +783,6 @@
     <t>LANGUAGES</t>
   </si>
   <si>
-    <t>en","da","kl</t>
-  </si>
-  <si>
     <t>MATRIX</t>
   </si>
   <si>
@@ -868,6 +865,9 @@
   </si>
   <si>
     <t>lexis a-grupper</t>
+  </si>
+  <si>
+    <t>en, da, kl</t>
   </si>
 </sst>
 </file>
@@ -1264,7 +1264,7 @@
   <dimension ref="A1:B40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1286,12 +1286,12 @@
         <v>249</v>
       </c>
       <c r="B2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B3" s="2">
         <v>2000</v>
@@ -1310,15 +1310,15 @@
         <v>252</v>
       </c>
       <c r="B5" t="s">
-        <v>253</v>
+        <v>281</v>
       </c>
     </row>
     <row r="6" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>253</v>
+      </c>
+      <c r="B6" t="s">
         <v>254</v>
-      </c>
-      <c r="B6" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1443,7 +1443,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B22" t="s">
         <v>206</v>
@@ -1451,7 +1451,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B23" t="s">
         <v>207</v>
@@ -1459,7 +1459,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B24" t="s">
         <v>208</v>
@@ -1467,7 +1467,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B25" t="s">
         <v>209</v>
@@ -1499,7 +1499,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B29" t="s">
         <v>213</v>
@@ -1507,7 +1507,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B30" t="s">
         <v>214</v>
@@ -1515,7 +1515,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B31" t="s">
         <v>215</v>
@@ -1523,15 +1523,15 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B32" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B33">
         <v>15</v>
@@ -1539,7 +1539,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -1630,16 +1630,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>276</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>277</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>1</v>
@@ -1729,7 +1729,7 @@
         <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D4" t="s">
         <v>25</v>
@@ -1825,7 +1825,7 @@
         <v>42</v>
       </c>
       <c r="C7" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D7" t="s">
         <v>43</v>
@@ -1880,16 +1880,16 @@
         <v>183</v>
       </c>
       <c r="C9" t="s">
+        <v>259</v>
+      </c>
+      <c r="D9" t="s">
+        <v>259</v>
+      </c>
+      <c r="E9" t="s">
         <v>260</v>
       </c>
-      <c r="D9" t="s">
-        <v>260</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>261</v>
-      </c>
-      <c r="F9" t="s">
-        <v>262</v>
       </c>
     </row>
   </sheetData>
@@ -1917,19 +1917,19 @@
   <sheetData>
     <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>53</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>279</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>280</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>54</v>
@@ -4154,7 +4154,7 @@
         <v>164</v>
       </c>
       <c r="D107" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E107" t="s">
         <v>165</v>

</xml_diff>

<commit_message>
Split 'position' into 'pivot' and 'order'
Close #124
</commit_message>
<xml_diff>
--- a/tests/testthat/fixtures/metadata/metadata_BEXLTALL.xlsx
+++ b/tests/testthat/fixtures/metadata/metadata_BEXLTALL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johan Ejstrud\Dropbox\repo\pxmake\tests\testthat\fixtures\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3418099B-B322-4E4B-AA4E-4F1E4AAD66ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E10B365-DE8F-4B47-9E88-99EEDB7D93DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31680" yWindow="10050" windowWidth="24210" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16680" yWindow="0" windowWidth="24210" windowHeight="31785" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="3" r:id="rId1"/>
@@ -22,10 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="282">
-  <si>
-    <t>position</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="277">
   <si>
     <t>type</t>
   </si>
@@ -57,9 +54,6 @@
     <t>kl_domain</t>
   </si>
   <si>
-    <t>h1</t>
-  </si>
-  <si>
     <t>time</t>
   </si>
   <si>
@@ -69,9 +63,6 @@
     <t>piffissaq</t>
   </si>
   <si>
-    <t>s1</t>
-  </si>
-  <si>
     <t>place of birth</t>
   </si>
   <si>
@@ -81,9 +72,6 @@
     <t>inunngorfik</t>
   </si>
   <si>
-    <t>2MD</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
@@ -93,9 +81,6 @@
     <t>Katillugit</t>
   </si>
   <si>
-    <t>s2</t>
-  </si>
-  <si>
     <t>nop</t>
   </si>
   <si>
@@ -114,9 +99,6 @@
     <t>kl 5 år</t>
   </si>
   <si>
-    <t>s3</t>
-  </si>
-  <si>
     <t>age</t>
   </si>
   <si>
@@ -138,18 +120,12 @@
     <t>VPUkiuian</t>
   </si>
   <si>
-    <t>s4</t>
-  </si>
-  <si>
     <t>køn</t>
   </si>
   <si>
     <t>suiaassuseq</t>
   </si>
   <si>
-    <t>s5</t>
-  </si>
-  <si>
     <t>calcbase</t>
   </si>
   <si>
@@ -162,9 +138,6 @@
     <t>kl b</t>
   </si>
   <si>
-    <t>s6</t>
-  </si>
-  <si>
     <t>measure</t>
   </si>
   <si>
@@ -807,9 +780,6 @@
     <t>amerlassusaat</t>
   </si>
   <si>
-    <t>FIGURES</t>
-  </si>
-  <si>
     <t>20230222 09:00</t>
   </si>
   <si>
@@ -868,6 +838,21 @@
   </si>
   <si>
     <t>en, da, kl</t>
+  </si>
+  <si>
+    <t>pivot</t>
+  </si>
+  <si>
+    <t>stub</t>
+  </si>
+  <si>
+    <t>heading</t>
+  </si>
+  <si>
+    <t>figures</t>
+  </si>
+  <si>
+    <t>order</t>
   </si>
 </sst>
 </file>
@@ -941,9 +926,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -981,9 +966,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1016,26 +1001,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1068,26 +1036,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1263,8 +1214,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1275,23 +1226,23 @@
   <sheetData>
     <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="B2" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
       <c r="B3" s="2">
         <v>2000</v>
@@ -1299,239 +1250,239 @@
     </row>
     <row r="4" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
       <c r="B4" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
     </row>
     <row r="5" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="B5" t="s">
-        <v>281</v>
+        <v>271</v>
       </c>
     </row>
     <row r="6" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="B6" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="B7" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="B8" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="B9" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="B10" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="B11" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="B12" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="B13" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="B14" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="B15" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="B16" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="B17" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="B18" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="B19" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="B20" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="B21" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="B22" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>266</v>
+        <v>256</v>
       </c>
       <c r="B23" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
       <c r="B24" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>268</v>
+        <v>258</v>
       </c>
       <c r="B25" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="B26" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="B27" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="B28" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
       <c r="B29" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="B30" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
       <c r="B31" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
       <c r="B32" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="B33">
         <v>15</v>
@@ -1539,7 +1490,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -1547,50 +1498,50 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="B35" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="B36" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="B37" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="B38" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="B39" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="B40" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -1600,296 +1551,302 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O9"/>
+  <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F70" sqref="F70"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>273</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="H1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>274</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>275</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>276</v>
-      </c>
-      <c r="F1" s="3" t="s">
+      <c r="B2">
         <v>1</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="O1" s="3" t="s">
+      <c r="C2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
         <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" t="s">
-        <v>14</v>
       </c>
       <c r="F2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>273</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L3" t="s">
+        <v>16</v>
+      </c>
+      <c r="M3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>273</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>249</v>
+      </c>
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" t="s">
+        <v>22</v>
+      </c>
+      <c r="L4" t="s">
+        <v>23</v>
+      </c>
+      <c r="M4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>273</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M5" t="s">
+        <v>28</v>
+      </c>
+      <c r="N5" t="s">
+        <v>29</v>
+      </c>
+      <c r="O5" t="s">
         <v>30</v>
       </c>
-      <c r="B3" t="s">
+      <c r="P5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>273</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>215</v>
+      </c>
+      <c r="D6" t="s">
+        <v>215</v>
+      </c>
+      <c r="E6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" t="s">
+        <v>33</v>
+      </c>
+      <c r="K6" t="s">
         <v>16</v>
       </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="L6" t="s">
         <v>17</v>
       </c>
-      <c r="E3" t="s">
+      <c r="M6" t="s">
         <v>18</v>
       </c>
-      <c r="F3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" t="s">
-        <v>20</v>
-      </c>
-      <c r="K3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" t="s">
-        <v>258</v>
-      </c>
-      <c r="D4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J4" t="s">
-        <v>27</v>
-      </c>
-      <c r="K4" t="s">
-        <v>28</v>
-      </c>
-      <c r="L4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>273</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" t="s">
+        <v>248</v>
+      </c>
+      <c r="E7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" t="s">
+        <v>36</v>
+      </c>
+      <c r="K7" t="s">
+        <v>158</v>
+      </c>
+      <c r="L7" t="s">
+        <v>159</v>
+      </c>
+      <c r="M7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>273</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" t="s">
+        <v>40</v>
+      </c>
+      <c r="K8" t="s">
         <v>41</v>
       </c>
-      <c r="B5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J5" t="s">
-        <v>34</v>
-      </c>
-      <c r="K5" t="s">
-        <v>34</v>
-      </c>
-      <c r="L5" t="s">
-        <v>34</v>
-      </c>
-      <c r="M5" t="s">
-        <v>35</v>
-      </c>
-      <c r="N5" t="s">
-        <v>36</v>
-      </c>
-      <c r="O5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6" t="s">
-        <v>224</v>
-      </c>
-      <c r="C6" t="s">
-        <v>224</v>
-      </c>
-      <c r="D6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E6" t="s">
-        <v>40</v>
-      </c>
-      <c r="F6" t="s">
-        <v>19</v>
-      </c>
-      <c r="J6" t="s">
-        <v>20</v>
-      </c>
-      <c r="K6" t="s">
-        <v>21</v>
-      </c>
-      <c r="L6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="L8" t="s">
         <v>42</v>
       </c>
-      <c r="C7" t="s">
-        <v>257</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="M8" t="s">
         <v>43</v>
       </c>
-      <c r="E7" t="s">
-        <v>44</v>
-      </c>
-      <c r="F7" t="s">
-        <v>19</v>
-      </c>
-      <c r="J7" t="s">
-        <v>167</v>
-      </c>
-      <c r="K7" t="s">
-        <v>168</v>
-      </c>
-      <c r="L7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>46</v>
-      </c>
-      <c r="B8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C8" t="s">
-        <v>47</v>
-      </c>
-      <c r="D8" t="s">
-        <v>48</v>
-      </c>
-      <c r="E8" t="s">
-        <v>49</v>
-      </c>
-      <c r="F8" t="s">
-        <v>19</v>
-      </c>
-      <c r="J8" t="s">
-        <v>50</v>
-      </c>
-      <c r="K8" t="s">
-        <v>51</v>
-      </c>
-      <c r="L8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>183</v>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>275</v>
       </c>
       <c r="C9" t="s">
-        <v>259</v>
+        <v>174</v>
       </c>
       <c r="D9" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="E9" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="F9" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
     </row>
   </sheetData>
@@ -1901,7 +1858,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G112"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G103" sqref="G103"/>
     </sheetView>
   </sheetViews>
@@ -1917,42 +1874,42 @@
   <sheetData>
     <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" t="s">
         <v>16</v>
       </c>
-      <c r="B2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C2" t="s">
-        <v>20</v>
-      </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -1961,19 +1918,19 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C3" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D3" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="E3" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="F3">
         <v>2</v>
@@ -1982,19 +1939,19 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="C4" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="D4" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="E4" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -2003,19 +1960,19 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="C5" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="D5" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="E5" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="F5">
         <v>2</v>
@@ -2024,19 +1981,19 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>224</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" t="s">
         <v>24</v>
-      </c>
-      <c r="B6" t="s">
-        <v>233</v>
-      </c>
-      <c r="C6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" t="s">
-        <v>29</v>
       </c>
       <c r="F6">
         <v>3</v>
@@ -2045,19 +2002,19 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="C7" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="D7" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="E7" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -2066,19 +2023,19 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="C8" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="D8" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="E8" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -2087,19 +2044,19 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="C9" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="D9" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E9" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="F9">
         <v>2</v>
@@ -2108,19 +2065,19 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B10" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="C10" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="D10" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="E10" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="F10">
         <v>3</v>
@@ -2129,19 +2086,19 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="C11" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="D11" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="E11" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="F11">
         <v>4</v>
@@ -2150,19 +2107,19 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B12" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="C12" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="D12" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="E12" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="F12">
         <v>5</v>
@@ -2171,19 +2128,19 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="C13" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="D13" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="E13" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="F13">
         <v>6</v>
@@ -2192,19 +2149,19 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C14" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="D14" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="E14" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="F14">
         <v>7</v>
@@ -2213,19 +2170,19 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="C15" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="D15" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="E15" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="F15">
         <v>8</v>
@@ -2234,19 +2191,19 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B16" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C16" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="D16" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="E16" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="F16">
         <v>9</v>
@@ -2255,19 +2212,19 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B17" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C17" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="D17" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="E17" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="F17">
         <v>10</v>
@@ -2276,19 +2233,19 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="C18" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="D18" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="E18" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="F18">
         <v>11</v>
@@ -2297,19 +2254,19 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="C19" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="D19" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="E19" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="F19">
         <v>12</v>
@@ -2318,19 +2275,19 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="C20" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="D20" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="E20" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="F20">
         <v>13</v>
@@ -2339,19 +2296,19 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="C21" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="D21" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="E21" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="F21">
         <v>14</v>
@@ -2360,19 +2317,19 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B22" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="C22" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="D22" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="E22" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="F22">
         <v>15</v>
@@ -2381,19 +2338,19 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B23" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C23" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="D23" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="E23" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F23">
         <v>16</v>
@@ -2402,19 +2359,19 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="C24" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D24" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="E24" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="F24">
         <v>17</v>
@@ -2423,19 +2380,19 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C25" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="D25" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="E25" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="F25">
         <v>18</v>
@@ -2444,19 +2401,19 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="C26" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="D26" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="E26" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="F26">
         <v>19</v>
@@ -2465,19 +2422,19 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="C27" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="D27" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E27" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="F27">
         <v>20</v>
@@ -2486,19 +2443,19 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B28" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="C28" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="D28" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="E28" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="F28">
         <v>21</v>
@@ -2507,19 +2464,19 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B29" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="C29" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="D29" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="E29" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="F29">
         <v>22</v>
@@ -2528,19 +2485,19 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B30" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="C30" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="D30" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="E30" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="F30">
         <v>23</v>
@@ -2549,19 +2506,19 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B31" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="C31" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="D31" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="E31" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="F31">
         <v>24</v>
@@ -2570,19 +2527,19 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B32" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C32" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="D32" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="E32" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="F32">
         <v>25</v>
@@ -2591,19 +2548,19 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B33" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="C33" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="D33" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="E33" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="F33">
         <v>26</v>
@@ -2612,19 +2569,19 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B34" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="C34" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="D34" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="E34" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="F34">
         <v>27</v>
@@ -2633,19 +2590,19 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B35" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="C35" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="D35" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="E35" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="F35">
         <v>28</v>
@@ -2654,19 +2611,19 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B36" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="C36" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="D36" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="E36" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="F36">
         <v>29</v>
@@ -2675,19 +2632,19 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B37" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="C37" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="D37" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="E37" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="F37">
         <v>30</v>
@@ -2696,19 +2653,19 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B38" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="C38" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="D38" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E38" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="F38">
         <v>31</v>
@@ -2717,19 +2674,19 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B39" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="C39" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="D39" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="E39" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="F39">
         <v>32</v>
@@ -2738,19 +2695,19 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B40" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="C40" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="D40" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="E40" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="F40">
         <v>33</v>
@@ -2759,19 +2716,19 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B41" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="C41" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="D41" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="E41" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="F41">
         <v>34</v>
@@ -2780,19 +2737,19 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B42" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="C42" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="D42" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="E42" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="F42">
         <v>35</v>
@@ -2801,19 +2758,19 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B43" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="C43" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="D43" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="E43" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="F43">
         <v>36</v>
@@ -2822,19 +2779,19 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B44" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C44" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="D44" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="E44" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="F44">
         <v>37</v>
@@ -2843,19 +2800,19 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B45" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="C45" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="D45" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="E45" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="F45">
         <v>38</v>
@@ -2864,19 +2821,19 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B46" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="C46" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="D46" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="E46" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="F46">
         <v>39</v>
@@ -2885,19 +2842,19 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B47" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="C47" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="D47" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="E47" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="F47">
         <v>40</v>
@@ -2906,19 +2863,19 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B48" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="C48" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="D48" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="E48" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="F48">
         <v>41</v>
@@ -2927,19 +2884,19 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B49" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="C49" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="D49" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="E49" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="F49">
         <v>42</v>
@@ -2948,19 +2905,19 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B50" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="C50" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="D50" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="E50" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="F50">
         <v>43</v>
@@ -2969,19 +2926,19 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B51" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="C51" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="D51" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="E51" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="F51">
         <v>44</v>
@@ -2990,19 +2947,19 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B52" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C52" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="D52" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="E52" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="F52">
         <v>45</v>
@@ -3011,19 +2968,19 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B53" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="C53" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="D53" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="E53" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="F53">
         <v>46</v>
@@ -3032,19 +2989,19 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B54" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="C54" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D54" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="E54" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="F54">
         <v>47</v>
@@ -3053,19 +3010,19 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B55" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="C55" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="D55" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="E55" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="F55">
         <v>48</v>
@@ -3074,19 +3031,19 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B56" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="C56" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="D56" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="E56" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="F56">
         <v>49</v>
@@ -3095,19 +3052,19 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B57" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="C57" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="D57" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="E57" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="F57">
         <v>50</v>
@@ -3116,19 +3073,19 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B58" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="C58" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="D58" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="E58" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="F58">
         <v>51</v>
@@ -3137,19 +3094,19 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B59" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="C59" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="D59" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="E59" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="F59">
         <v>52</v>
@@ -3158,19 +3115,19 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B60" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="C60" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="D60" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="E60" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="F60">
         <v>53</v>
@@ -3179,19 +3136,19 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B61" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="C61" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="D61" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="E61" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="F61">
         <v>54</v>
@@ -3200,19 +3157,19 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B62" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="C62" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="D62" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="E62" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="F62">
         <v>55</v>
@@ -3221,19 +3178,19 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B63" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="C63" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="D63" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="E63" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="F63">
         <v>56</v>
@@ -3242,19 +3199,19 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B64" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="C64" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="D64" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="E64" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="F64">
         <v>57</v>
@@ -3263,19 +3220,19 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B65" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="C65" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="D65" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="E65" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="F65">
         <v>58</v>
@@ -3284,19 +3241,19 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B66" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="C66" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="D66" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="E66" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="F66">
         <v>59</v>
@@ -3305,19 +3262,19 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B67" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="C67" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="D67" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="E67" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="F67">
         <v>60</v>
@@ -3326,19 +3283,19 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B68" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="C68" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="D68" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="E68" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="F68">
         <v>61</v>
@@ -3347,19 +3304,19 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B69" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="C69" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="D69" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="E69" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="F69">
         <v>62</v>
@@ -3368,19 +3325,19 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B70" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="C70" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="D70" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="E70" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="F70">
         <v>63</v>
@@ -3389,19 +3346,19 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B71" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="C71" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="D71" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="E71" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="F71">
         <v>64</v>
@@ -3410,19 +3367,19 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B72" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="C72" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="D72" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="E72" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="F72">
         <v>65</v>
@@ -3431,19 +3388,19 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B73" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="C73" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="D73" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="E73" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="F73">
         <v>66</v>
@@ -3452,19 +3409,19 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B74" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="C74" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="D74" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="E74" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="F74">
         <v>67</v>
@@ -3473,19 +3430,19 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B75" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="C75" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="D75" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="E75" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="F75">
         <v>68</v>
@@ -3494,19 +3451,19 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B76" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="C76" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="D76" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="E76" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="F76">
         <v>69</v>
@@ -3515,19 +3472,19 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B77" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="C77" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="D77" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="E77" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="F77">
         <v>70</v>
@@ -3536,19 +3493,19 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B78" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="C78" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="D78" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="E78" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="F78">
         <v>71</v>
@@ -3557,19 +3514,19 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B79" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="C79" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="D79" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E79" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="F79">
         <v>72</v>
@@ -3578,19 +3535,19 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B80" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="C80" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="D80" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="E80" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="F80">
         <v>73</v>
@@ -3599,19 +3556,19 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B81" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="C81" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="D81" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="E81" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="F81">
         <v>74</v>
@@ -3620,19 +3577,19 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B82" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="C82" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="D82" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="E82" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="F82">
         <v>75</v>
@@ -3641,19 +3598,19 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B83" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="C83" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="D83" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="E83" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="F83">
         <v>76</v>
@@ -3662,19 +3619,19 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B84" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="C84" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="D84" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="E84" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="F84">
         <v>77</v>
@@ -3683,19 +3640,19 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B85" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="C85" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="D85" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="E85" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="F85">
         <v>78</v>
@@ -3704,19 +3661,19 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B86" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="C86" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="D86" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="E86" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="F86">
         <v>79</v>
@@ -3725,19 +3682,19 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B87" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C87" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="D87" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="E87" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="F87">
         <v>80</v>
@@ -3746,19 +3703,19 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B88" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="C88" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="D88" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="E88" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="F88">
         <v>81</v>
@@ -3767,19 +3724,19 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B89" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="C89" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="D89" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="E89" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="F89">
         <v>82</v>
@@ -3788,19 +3745,19 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B90" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="C90" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="D90" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="E90" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="F90">
         <v>83</v>
@@ -3809,19 +3766,19 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B91" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="C91" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="D91" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="E91" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="F91">
         <v>84</v>
@@ -3830,19 +3787,19 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B92" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="C92" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="D92" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="E92" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="F92">
         <v>85</v>
@@ -3851,19 +3808,19 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B93" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="C93" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="D93" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="E93" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="F93">
         <v>86</v>
@@ -3872,19 +3829,19 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B94" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="C94" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="D94" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="E94" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="F94">
         <v>87</v>
@@ -3893,19 +3850,19 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B95" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="C95" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="D95" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="E95" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="F95">
         <v>88</v>
@@ -3914,19 +3871,19 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B96" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="C96" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="D96" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="E96" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="F96">
         <v>89</v>
@@ -3935,19 +3892,19 @@
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B97" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="C97" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D97" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="E97" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="F97">
         <v>90</v>
@@ -3956,19 +3913,19 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B98" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="C98" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="D98" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="E98" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="F98">
         <v>91</v>
@@ -3977,19 +3934,19 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B99" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="C99" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="D99" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="E99" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="F99">
         <v>92</v>
@@ -3998,19 +3955,19 @@
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B100" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="C100" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="D100" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="E100" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="F100">
         <v>93</v>
@@ -4019,19 +3976,19 @@
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B101" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="C101" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="D101" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="E101" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="F101">
         <v>94</v>
@@ -4040,19 +3997,19 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B102" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="C102" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="D102" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="E102" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="F102">
         <v>95</v>
@@ -4061,7 +4018,7 @@
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B103">
         <v>99</v>
@@ -4082,19 +4039,19 @@
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="B104" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="C104" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D104" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E104" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F104">
         <v>1</v>
@@ -4103,19 +4060,19 @@
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="B105" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="C105" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="D105" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="E105" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="F105">
         <v>2</v>
@@ -4124,19 +4081,19 @@
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="B106" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="C106" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="D106" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="E106" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="F106">
         <v>3</v>
@@ -4145,19 +4102,19 @@
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B107" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="C107" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="D107" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="E107" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="F107">
         <v>1</v>
@@ -4166,19 +4123,19 @@
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B108" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="C108" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="D108" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="E108" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="F108">
         <v>2</v>
@@ -4187,65 +4144,65 @@
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="B109" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="C109" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="D109" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="E109" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="F109">
         <v>1</v>
       </c>
       <c r="G109" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="B110" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="C110" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="D110" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="E110" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="F110">
         <v>2</v>
       </c>
       <c r="G110" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="B111" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="C111" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="D111" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="E111" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="F111">
         <v>3</v>
@@ -4253,25 +4210,25 @@
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="B112" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="C112" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="D112" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="E112" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="F112">
         <v>4</v>
       </c>
       <c r="G112" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rename 'variable' and 'long_name' to 'variable-code' and 'variable-label'
Close #144
</commit_message>
<xml_diff>
--- a/tests/testthat/fixtures/metadata/metadata_BEXLTALL.xlsx
+++ b/tests/testthat/fixtures/metadata/metadata_BEXLTALL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johan Ejstrud\Dropbox\repo\pxmake\tests\testthat\fixtures\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E10B365-DE8F-4B47-9E88-99EEDB7D93DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49505C85-8C27-4C41-A8CE-1B6D376F2488}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16680" yWindow="0" windowWidth="24210" windowHeight="31785" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3810" yWindow="3810" windowWidth="24210" windowHeight="21645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="3" r:id="rId1"/>
@@ -813,27 +813,6 @@
     <t>NEXT-UPDATE</t>
   </si>
   <si>
-    <t>variable</t>
-  </si>
-  <si>
-    <t>en_long_name</t>
-  </si>
-  <si>
-    <t>da_long_name</t>
-  </si>
-  <si>
-    <t>kl_long_name</t>
-  </si>
-  <si>
-    <t>en_code_label</t>
-  </si>
-  <si>
-    <t>da_code_label</t>
-  </si>
-  <si>
-    <t>kl_code_label</t>
-  </si>
-  <si>
     <t>lexis a-grupper</t>
   </si>
   <si>
@@ -853,6 +832,27 @@
   </si>
   <si>
     <t>order</t>
+  </si>
+  <si>
+    <t>variable-code</t>
+  </si>
+  <si>
+    <t>en_code-label</t>
+  </si>
+  <si>
+    <t>da_code-label</t>
+  </si>
+  <si>
+    <t>kl_code-label</t>
+  </si>
+  <si>
+    <t>en_variable-label</t>
+  </si>
+  <si>
+    <t>da_variable-label</t>
+  </si>
+  <si>
+    <t>kl_variable-label</t>
   </si>
 </sst>
 </file>
@@ -1261,7 +1261,7 @@
         <v>243</v>
       </c>
       <c r="B5" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
     </row>
     <row r="6" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1554,7 +1554,7 @@
   <dimension ref="A1:P9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1578,22 +1578,22 @@
   <sheetData>
     <row r="1" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>276</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>264</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>265</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>266</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>0</v>
@@ -1628,7 +1628,7 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1651,7 +1651,7 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -1680,7 +1680,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -1709,7 +1709,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="B5">
         <v>5</v>
@@ -1747,7 +1747,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="B6">
         <v>4</v>
@@ -1776,7 +1776,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -1805,7 +1805,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="B8">
         <v>6</v>
@@ -1834,7 +1834,7 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="C9" t="s">
         <v>174</v>
@@ -1859,7 +1859,7 @@
   <dimension ref="A1:G112"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G103" sqref="G103"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1874,19 +1874,19 @@
   <sheetData>
     <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>263</v>
+        <v>270</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>44</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>45</v>
@@ -4111,7 +4111,7 @@
         <v>155</v>
       </c>
       <c r="D107" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="E107" t="s">
         <v>156</v>

</xml_diff>

<commit_message>
Rename 'codelists' to 'cells'
Close #256
</commit_message>
<xml_diff>
--- a/tests/testthat/fixtures/metadata/metadata_BEXLTALL.xlsx
+++ b/tests/testthat/fixtures/metadata/metadata_BEXLTALL.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johan Ejstrud\Dropbox\repo\pxmake\tests\testthat\fixtures\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63E6D683-4AA7-4C7A-98BC-AF4A76165180}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{501162BD-0FC7-4698-9BA5-E88F73DBA2C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16995" windowHeight="31680" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="41595" yWindow="11685" windowWidth="15450" windowHeight="13425" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
     <sheet name="Table2" sheetId="2" r:id="rId2"/>
     <sheet name="Variables" sheetId="3" r:id="rId3"/>
-    <sheet name="Codelists" sheetId="4" r:id="rId4"/>
+    <sheet name="Cells" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -1826,7 +1826,7 @@
   <dimension ref="A1:G112"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Rename 'type' to 'variables-type
</commit_message>
<xml_diff>
--- a/tests/testthat/fixtures/metadata/metadata_BEXLTALL.xlsx
+++ b/tests/testthat/fixtures/metadata/metadata_BEXLTALL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johan Ejstrud\Dropbox\repo\pxmake\tests\testthat\fixtures\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{501162BD-0FC7-4698-9BA5-E88F73DBA2C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39B6D23C-E23B-4E18-ADF4-67EFC76BC862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41595" yWindow="11685" windowWidth="15450" windowHeight="13425" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6240" yWindow="6240" windowWidth="15450" windowHeight="13425" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -220,9 +220,6 @@
     <t>variable-code</t>
   </si>
   <si>
-    <t>type</t>
-  </si>
-  <si>
     <t>en_variable-label</t>
   </si>
   <si>
@@ -812,6 +809,9 @@
   </si>
   <si>
     <t>Arnat</t>
+  </si>
+  <si>
+    <t>variable-type</t>
   </si>
 </sst>
 </file>
@@ -898,7 +898,7 @@
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="pivot"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="order"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="variable-code"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="type"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="variable-type"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="en_variable-label"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="da_variable-label"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="kl_variable-label"/>
@@ -1515,15 +1515,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" customWidth="1"/>
     <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
@@ -1550,266 +1550,266 @@
         <v>64</v>
       </c>
       <c r="D1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E1" t="s">
         <v>65</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>66</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>67</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>68</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>69</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>70</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>71</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>72</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>73</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>74</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>75</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>76</v>
-      </c>
-      <c r="P1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B2">
         <v>5</v>
       </c>
       <c r="C2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" t="s">
         <v>79</v>
       </c>
-      <c r="E2" t="s">
-        <v>79</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>80</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>81</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>82</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>83</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>84</v>
       </c>
-      <c r="K2" t="s">
-        <v>85</v>
-      </c>
       <c r="L2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="M2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E3" t="s">
         <v>86</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>87</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>88</v>
       </c>
-      <c r="G3" t="s">
+      <c r="K3" t="s">
         <v>89</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>90</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>91</v>
-      </c>
-      <c r="M3" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B4">
         <v>6</v>
       </c>
       <c r="C4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F4" t="s">
         <v>93</v>
       </c>
-      <c r="E4" t="s">
-        <v>93</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>94</v>
       </c>
-      <c r="G4" t="s">
+      <c r="K4" t="s">
         <v>95</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>96</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>97</v>
-      </c>
-      <c r="M4" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B5">
         <v>2</v>
       </c>
       <c r="C5" t="s">
+        <v>98</v>
+      </c>
+      <c r="E5" t="s">
         <v>99</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>100</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>101</v>
       </c>
-      <c r="G5" t="s">
+      <c r="K5" t="s">
         <v>102</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>103</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>104</v>
-      </c>
-      <c r="M5" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B6">
         <v>3</v>
       </c>
       <c r="C6" t="s">
+        <v>105</v>
+      </c>
+      <c r="E6" t="s">
+        <v>105</v>
+      </c>
+      <c r="F6" t="s">
         <v>106</v>
       </c>
-      <c r="E6" t="s">
-        <v>106</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>107</v>
       </c>
-      <c r="G6" t="s">
+      <c r="K6" t="s">
         <v>108</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
+        <v>108</v>
+      </c>
+      <c r="M6" t="s">
         <v>109</v>
-      </c>
-      <c r="L6" t="s">
-        <v>109</v>
-      </c>
-      <c r="M6" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B7">
         <v>4</v>
       </c>
       <c r="C7" t="s">
+        <v>110</v>
+      </c>
+      <c r="E7" t="s">
+        <v>110</v>
+      </c>
+      <c r="F7" t="s">
         <v>111</v>
       </c>
-      <c r="E7" t="s">
-        <v>111</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>112</v>
       </c>
-      <c r="G7" t="s">
+      <c r="K7" t="s">
+        <v>108</v>
+      </c>
+      <c r="L7" t="s">
         <v>113</v>
       </c>
-      <c r="K7" t="s">
+      <c r="M7" t="s">
         <v>109</v>
-      </c>
-      <c r="L7" t="s">
-        <v>114</v>
-      </c>
-      <c r="M7" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" t="s">
+        <v>115</v>
+      </c>
+      <c r="D8" t="s">
         <v>116</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
+        <v>115</v>
+      </c>
+      <c r="F8" t="s">
         <v>117</v>
       </c>
-      <c r="E8" t="s">
-        <v>116</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>118</v>
-      </c>
-      <c r="G8" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C9" t="s">
         <v>1</v>
       </c>
       <c r="E9" t="s">
+        <v>120</v>
+      </c>
+      <c r="F9" t="s">
+        <v>120</v>
+      </c>
+      <c r="G9" t="s">
         <v>121</v>
-      </c>
-      <c r="F9" t="s">
-        <v>121</v>
-      </c>
-      <c r="G9" t="s">
-        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -1825,7 +1825,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G112"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
@@ -1848,24 +1848,24 @@
         <v>24</v>
       </c>
       <c r="C1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D1" t="s">
         <v>123</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>124</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>125</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>126</v>
-      </c>
-      <c r="G1" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B2" t="s">
         <v>19</v>
@@ -1885,287 +1885,287 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C7">
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C8">
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C9">
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C10">
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C11">
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C12">
         <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C13">
         <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C14">
         <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B15" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C15">
         <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E15" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F15" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C16">
         <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B17" t="s">
         <v>17</v>
@@ -2185,1911 +2185,1911 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C18">
         <v>17</v>
       </c>
       <c r="D18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B19" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C19">
         <v>18</v>
       </c>
       <c r="D19" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E19" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F19" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B20" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C20">
         <v>19</v>
       </c>
       <c r="D20" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E20" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F20" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B21" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C21">
         <v>20</v>
       </c>
       <c r="D21" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E21" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F21" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C22">
         <v>21</v>
       </c>
       <c r="D22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B23" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C23">
         <v>22</v>
       </c>
       <c r="D23" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E23" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F23" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B24" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C24">
         <v>23</v>
       </c>
       <c r="D24" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E24" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F24" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B25" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C25">
         <v>24</v>
       </c>
       <c r="D25" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E25" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F25" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B26" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C26">
         <v>25</v>
       </c>
       <c r="D26" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E26" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F26" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B27" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C27">
         <v>26</v>
       </c>
       <c r="D27" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E27" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F27" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B28" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C28">
         <v>27</v>
       </c>
       <c r="D28" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E28" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F28" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B29" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C29">
         <v>28</v>
       </c>
       <c r="D29" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E29" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F29" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B30" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C30">
         <v>29</v>
       </c>
       <c r="D30" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E30" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F30" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B31" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C31">
         <v>30</v>
       </c>
       <c r="D31" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E31" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F31" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B32" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C32">
         <v>31</v>
       </c>
       <c r="D32" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E32" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F32" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B33" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C33">
         <v>32</v>
       </c>
       <c r="D33" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E33" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F33" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B34" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C34">
         <v>33</v>
       </c>
       <c r="D34" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E34" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F34" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B35" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C35">
         <v>34</v>
       </c>
       <c r="D35" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E35" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F35" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B36" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C36">
         <v>35</v>
       </c>
       <c r="D36" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E36" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F36" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B37" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C37">
         <v>36</v>
       </c>
       <c r="D37" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E37" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F37" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B38" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C38">
         <v>37</v>
       </c>
       <c r="D38" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E38" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F38" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B39" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C39">
         <v>38</v>
       </c>
       <c r="D39" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E39" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F39" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C40">
         <v>39</v>
       </c>
       <c r="D40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B41" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C41">
         <v>40</v>
       </c>
       <c r="D41" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E41" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F41" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B42" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C42">
         <v>41</v>
       </c>
       <c r="D42" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E42" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F42" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B43" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C43">
         <v>42</v>
       </c>
       <c r="D43" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E43" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F43" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B44" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C44">
         <v>43</v>
       </c>
       <c r="D44" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E44" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F44" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B45" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C45">
         <v>44</v>
       </c>
       <c r="D45" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E45" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F45" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B46" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C46">
         <v>45</v>
       </c>
       <c r="D46" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E46" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F46" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B47" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C47">
         <v>46</v>
       </c>
       <c r="D47" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E47" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F47" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B48" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C48">
         <v>47</v>
       </c>
       <c r="D48" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E48" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F48" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B49" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C49">
         <v>48</v>
       </c>
       <c r="D49" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E49" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F49" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B50" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C50">
         <v>49</v>
       </c>
       <c r="D50" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E50" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F50" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B51" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C51">
         <v>50</v>
       </c>
       <c r="D51" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E51" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F51" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B52" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C52">
         <v>51</v>
       </c>
       <c r="D52" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E52" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F52" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B53" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C53">
         <v>52</v>
       </c>
       <c r="D53" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E53" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F53" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B54" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C54">
         <v>53</v>
       </c>
       <c r="D54" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E54" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F54" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B55" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C55">
         <v>54</v>
       </c>
       <c r="D55" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E55" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F55" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B56" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C56">
         <v>55</v>
       </c>
       <c r="D56" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E56" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F56" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B57" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C57">
         <v>56</v>
       </c>
       <c r="D57" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E57" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F57" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B58" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C58">
         <v>57</v>
       </c>
       <c r="D58" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E58" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F58" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B59" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C59">
         <v>58</v>
       </c>
       <c r="D59" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E59" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F59" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B60" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C60">
         <v>59</v>
       </c>
       <c r="D60" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E60" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F60" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B61" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C61">
         <v>60</v>
       </c>
       <c r="D61" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E61" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F61" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B62" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C62">
         <v>61</v>
       </c>
       <c r="D62" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E62" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F62" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B63" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C63">
         <v>62</v>
       </c>
       <c r="D63" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E63" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F63" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B64" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C64">
         <v>63</v>
       </c>
       <c r="D64" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E64" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F64" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B65" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C65">
         <v>64</v>
       </c>
       <c r="D65" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E65" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F65" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B66" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C66">
         <v>65</v>
       </c>
       <c r="D66" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E66" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F66" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B67" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C67">
         <v>66</v>
       </c>
       <c r="D67" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E67" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F67" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B68" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C68">
         <v>67</v>
       </c>
       <c r="D68" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E68" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F68" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B69" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C69">
         <v>68</v>
       </c>
       <c r="D69" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E69" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F69" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B70" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C70">
         <v>69</v>
       </c>
       <c r="D70" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E70" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F70" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B71" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C71">
         <v>70</v>
       </c>
       <c r="D71" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E71" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F71" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B72" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C72">
         <v>71</v>
       </c>
       <c r="D72" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E72" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F72" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B73" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C73">
         <v>72</v>
       </c>
       <c r="D73" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E73" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F73" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B74" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C74">
         <v>73</v>
       </c>
       <c r="D74" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E74" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F74" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B75" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C75">
         <v>74</v>
       </c>
       <c r="D75" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E75" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F75" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B76" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C76">
         <v>75</v>
       </c>
       <c r="D76" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E76" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F76" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B77" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C77">
         <v>76</v>
       </c>
       <c r="D77" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E77" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F77" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B78" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C78">
         <v>77</v>
       </c>
       <c r="D78" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E78" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F78" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C79">
         <v>78</v>
       </c>
       <c r="D79" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E79" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F79" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B80" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C80">
         <v>79</v>
       </c>
       <c r="D80" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E80" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F80" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B81" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C81">
         <v>80</v>
       </c>
       <c r="D81" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E81" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F81" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B82" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C82">
         <v>81</v>
       </c>
       <c r="D82" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E82" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F82" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B83" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C83">
         <v>82</v>
       </c>
       <c r="D83" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E83" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F83" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B84" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C84">
         <v>83</v>
       </c>
       <c r="D84" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E84" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F84" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B85" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C85">
         <v>84</v>
       </c>
       <c r="D85" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E85" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F85" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B86" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C86">
         <v>85</v>
       </c>
       <c r="D86" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E86" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F86" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B87" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C87">
         <v>86</v>
       </c>
       <c r="D87" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E87" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F87" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B88" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C88">
         <v>87</v>
       </c>
       <c r="D88" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E88" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F88" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B89" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C89">
         <v>88</v>
       </c>
       <c r="D89" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E89" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F89" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B90" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C90">
         <v>89</v>
       </c>
       <c r="D90" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E90" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F90" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B91" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C91">
         <v>90</v>
       </c>
       <c r="D91" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E91" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F91" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B92" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C92">
         <v>91</v>
       </c>
       <c r="D92" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E92" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F92" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B93" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C93">
         <v>92</v>
       </c>
       <c r="D93" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E93" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F93" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B94" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C94">
         <v>93</v>
       </c>
       <c r="D94" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E94" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F94" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B95" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C95">
         <v>94</v>
       </c>
       <c r="D95" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E95" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F95" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B96" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C96">
         <v>95</v>
       </c>
       <c r="D96" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E96" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F96" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B97" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C97">
         <v>96</v>
       </c>
       <c r="D97" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E97" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F97" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B98" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C98">
         <v>97</v>
       </c>
       <c r="D98" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E98" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F98" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B99" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C99">
         <v>1</v>
       </c>
       <c r="D99" t="s">
+        <v>223</v>
+      </c>
+      <c r="E99" t="s">
         <v>224</v>
       </c>
-      <c r="E99" t="s">
+      <c r="F99" t="s">
         <v>225</v>
-      </c>
-      <c r="F99" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B100" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C100">
         <v>2</v>
       </c>
       <c r="D100" t="s">
+        <v>89</v>
+      </c>
+      <c r="E100" t="s">
         <v>90</v>
       </c>
-      <c r="E100" t="s">
+      <c r="F100" t="s">
         <v>91</v>
-      </c>
-      <c r="F100" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B101" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C101">
         <v>1</v>
       </c>
       <c r="D101" t="s">
+        <v>228</v>
+      </c>
+      <c r="E101" t="s">
         <v>229</v>
       </c>
-      <c r="E101" t="s">
+      <c r="F101" t="s">
         <v>230</v>
       </c>
-      <c r="F101" t="s">
-        <v>231</v>
-      </c>
       <c r="G101" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B102" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C102">
         <v>2</v>
       </c>
       <c r="D102" t="s">
+        <v>232</v>
+      </c>
+      <c r="E102" t="s">
         <v>233</v>
       </c>
-      <c r="E102" t="s">
+      <c r="F102" t="s">
         <v>234</v>
       </c>
-      <c r="F102" t="s">
-        <v>235</v>
-      </c>
       <c r="G102" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B103" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C103">
         <v>3</v>
       </c>
       <c r="D103" t="s">
+        <v>236</v>
+      </c>
+      <c r="E103" t="s">
         <v>237</v>
       </c>
-      <c r="E103" t="s">
+      <c r="F103" t="s">
         <v>238</v>
-      </c>
-      <c r="F103" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B104" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C104">
         <v>4</v>
       </c>
       <c r="D104" t="s">
+        <v>95</v>
+      </c>
+      <c r="E104" t="s">
         <v>96</v>
       </c>
-      <c r="E104" t="s">
+      <c r="F104" t="s">
         <v>97</v>
       </c>
-      <c r="F104" t="s">
-        <v>98</v>
-      </c>
       <c r="G104" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B105" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C105">
         <v>1</v>
       </c>
       <c r="D105" t="s">
+        <v>241</v>
+      </c>
+      <c r="E105" t="s">
         <v>242</v>
       </c>
-      <c r="E105" t="s">
+      <c r="F105" t="s">
         <v>243</v>
-      </c>
-      <c r="F105" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B106" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C106">
         <v>2</v>
       </c>
       <c r="D106" t="s">
+        <v>245</v>
+      </c>
+      <c r="E106" t="s">
         <v>246</v>
       </c>
-      <c r="E106" t="s">
+      <c r="F106" t="s">
         <v>247</v>
-      </c>
-      <c r="F106" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B107" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C107">
         <v>3</v>
       </c>
       <c r="D107" t="s">
+        <v>102</v>
+      </c>
+      <c r="E107" t="s">
         <v>103</v>
       </c>
-      <c r="E107" t="s">
+      <c r="F107" t="s">
         <v>104</v>
-      </c>
-      <c r="F107" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B108" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C108">
         <v>1</v>
       </c>
       <c r="D108" t="s">
+        <v>108</v>
+      </c>
+      <c r="E108" t="s">
+        <v>108</v>
+      </c>
+      <c r="F108" t="s">
         <v>109</v>
-      </c>
-      <c r="E108" t="s">
-        <v>109</v>
-      </c>
-      <c r="F108" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B109" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C109">
         <v>2</v>
       </c>
       <c r="D109" t="s">
+        <v>251</v>
+      </c>
+      <c r="E109" t="s">
         <v>252</v>
       </c>
-      <c r="E109" t="s">
+      <c r="F109" t="s">
         <v>253</v>
-      </c>
-      <c r="F109" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B110" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C110">
         <v>1</v>
       </c>
       <c r="D110" t="s">
+        <v>108</v>
+      </c>
+      <c r="E110" t="s">
+        <v>113</v>
+      </c>
+      <c r="F110" t="s">
         <v>109</v>
-      </c>
-      <c r="E110" t="s">
-        <v>114</v>
-      </c>
-      <c r="F110" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B111" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C111">
         <v>2</v>
       </c>
       <c r="D111" t="s">
+        <v>255</v>
+      </c>
+      <c r="E111" t="s">
         <v>256</v>
       </c>
-      <c r="E111" t="s">
+      <c r="F111" t="s">
         <v>257</v>
-      </c>
-      <c r="F111" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B112" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C112">
         <v>3</v>
       </c>
       <c r="D112" t="s">
+        <v>259</v>
+      </c>
+      <c r="E112" t="s">
         <v>260</v>
       </c>
-      <c r="E112" t="s">
+      <c r="F112" t="s">
         <v>261</v>
-      </c>
-      <c r="F112" t="s">
-        <v>262</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Make a seperate column for TIMEVAL in variables1
Close #265
</commit_message>
<xml_diff>
--- a/tests/testthat/fixtures/metadata/metadata_BEXLTALL.xlsx
+++ b/tests/testthat/fixtures/metadata/metadata_BEXLTALL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johan Ejstrud\Dropbox\repo\pxmake\tests\testthat\fixtures\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39B6D23C-E23B-4E18-ADF4-67EFC76BC862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E530AFCA-C9C2-49D5-BFD5-6062E5C8692F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6240" yWindow="6240" windowWidth="15450" windowHeight="13425" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19005" yWindow="3960" windowWidth="15450" windowHeight="13425" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -373,9 +373,6 @@
     <t>time</t>
   </si>
   <si>
-    <t>TIME</t>
-  </si>
-  <si>
     <t>tid</t>
   </si>
   <si>
@@ -812,6 +809,9 @@
   </si>
   <si>
     <t>variable-type</t>
+  </si>
+  <si>
+    <t>timeval</t>
   </si>
 </sst>
 </file>
@@ -892,13 +892,14 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table5" displayName="Table5" ref="A1:P9" totalsRowShown="0">
-  <autoFilter ref="A1:P9" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
-  <tableColumns count="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table5" displayName="Table5" ref="A1:Q9" totalsRowShown="0">
+  <autoFilter ref="A1:Q9" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
+  <tableColumns count="17">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="pivot"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="order"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="variable-code"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="variable-type"/>
+    <tableColumn id="17" xr3:uid="{1F674A62-667E-4B54-9697-04C2424B310A}" name="timeval"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="en_variable-label"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="da_variable-label"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="kl_variable-label"/>
@@ -1513,10 +1514,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:P9"/>
+  <dimension ref="A1:Q9"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1525,21 +1526,22 @@
     <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.5703125" customWidth="1"/>
     <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.28515625" customWidth="1"/>
+    <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>62</v>
       </c>
@@ -1550,46 +1552,49 @@
         <v>64</v>
       </c>
       <c r="D1" t="s">
+        <v>261</v>
+      </c>
+      <c r="E1" t="s">
         <v>262</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>65</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>66</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>67</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>68</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>69</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>70</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>71</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>72</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>73</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>74</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>75</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>77</v>
       </c>
@@ -1599,26 +1604,23 @@
       <c r="C2" t="s">
         <v>78</v>
       </c>
-      <c r="E2" t="s">
-        <v>78</v>
-      </c>
       <c r="F2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G2" t="s">
         <v>79</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>80</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>81</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>82</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>83</v>
-      </c>
-      <c r="K2" t="s">
-        <v>84</v>
       </c>
       <c r="L2" t="s">
         <v>84</v>
@@ -1626,8 +1628,11 @@
       <c r="M2" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>77</v>
       </c>
@@ -1637,26 +1642,26 @@
       <c r="C3" t="s">
         <v>85</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>86</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>87</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>88</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>89</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>90</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>77</v>
       </c>
@@ -1666,26 +1671,26 @@
       <c r="C4" t="s">
         <v>92</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>92</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>93</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>94</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>95</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>96</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>77</v>
       </c>
@@ -1695,26 +1700,26 @@
       <c r="C5" t="s">
         <v>98</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>99</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>100</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>101</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>102</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>103</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>77</v>
       </c>
@@ -1724,26 +1729,26 @@
       <c r="C6" t="s">
         <v>105</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>105</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>106</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>107</v>
-      </c>
-      <c r="K6" t="s">
-        <v>108</v>
       </c>
       <c r="L6" t="s">
         <v>108</v>
       </c>
       <c r="M6" t="s">
+        <v>108</v>
+      </c>
+      <c r="N6" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>77</v>
       </c>
@@ -1753,26 +1758,26 @@
       <c r="C7" t="s">
         <v>110</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>110</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>111</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>112</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>108</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>113</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>114</v>
       </c>
@@ -1782,34 +1787,34 @@
       <c r="C8" t="s">
         <v>115</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F8" t="s">
+        <v>115</v>
+      </c>
+      <c r="G8" t="s">
         <v>116</v>
       </c>
-      <c r="E8" t="s">
-        <v>115</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="H8" t="s">
         <v>117</v>
       </c>
-      <c r="G8" t="s">
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>118</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>119</v>
       </c>
       <c r="C9" t="s">
         <v>1</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
+        <v>119</v>
+      </c>
+      <c r="G9" t="s">
+        <v>119</v>
+      </c>
+      <c r="H9" t="s">
         <v>120</v>
-      </c>
-      <c r="F9" t="s">
-        <v>120</v>
-      </c>
-      <c r="G9" t="s">
-        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -1848,19 +1853,19 @@
         <v>24</v>
       </c>
       <c r="C1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D1" t="s">
         <v>122</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>123</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>124</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>125</v>
-      </c>
-      <c r="G1" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1888,19 +1893,19 @@
         <v>78</v>
       </c>
       <c r="B3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1908,19 +1913,19 @@
         <v>78</v>
       </c>
       <c r="B4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1928,19 +1933,19 @@
         <v>78</v>
       </c>
       <c r="B5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1948,19 +1953,19 @@
         <v>78</v>
       </c>
       <c r="B6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1968,19 +1973,19 @@
         <v>78</v>
       </c>
       <c r="B7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C7">
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1988,19 +1993,19 @@
         <v>78</v>
       </c>
       <c r="B8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C8">
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -2008,19 +2013,19 @@
         <v>78</v>
       </c>
       <c r="B9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C9">
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -2028,19 +2033,19 @@
         <v>78</v>
       </c>
       <c r="B10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C10">
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -2048,19 +2053,19 @@
         <v>78</v>
       </c>
       <c r="B11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C11">
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -2068,19 +2073,19 @@
         <v>78</v>
       </c>
       <c r="B12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C12">
         <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -2088,19 +2093,19 @@
         <v>78</v>
       </c>
       <c r="B13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C13">
         <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -2108,19 +2113,19 @@
         <v>78</v>
       </c>
       <c r="B14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C14">
         <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -2128,19 +2133,19 @@
         <v>78</v>
       </c>
       <c r="B15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C15">
         <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -2148,19 +2153,19 @@
         <v>78</v>
       </c>
       <c r="B16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C16">
         <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -2188,19 +2193,19 @@
         <v>78</v>
       </c>
       <c r="B18" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C18">
         <v>17</v>
       </c>
       <c r="D18" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E18" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F18" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -2208,19 +2213,19 @@
         <v>78</v>
       </c>
       <c r="B19" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C19">
         <v>18</v>
       </c>
       <c r="D19" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E19" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F19" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -2228,19 +2233,19 @@
         <v>78</v>
       </c>
       <c r="B20" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C20">
         <v>19</v>
       </c>
       <c r="D20" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E20" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F20" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -2248,19 +2253,19 @@
         <v>78</v>
       </c>
       <c r="B21" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C21">
         <v>20</v>
       </c>
       <c r="D21" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E21" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F21" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -2268,19 +2273,19 @@
         <v>78</v>
       </c>
       <c r="B22" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C22">
         <v>21</v>
       </c>
       <c r="D22" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E22" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F22" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -2288,19 +2293,19 @@
         <v>78</v>
       </c>
       <c r="B23" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C23">
         <v>22</v>
       </c>
       <c r="D23" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E23" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F23" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -2308,19 +2313,19 @@
         <v>78</v>
       </c>
       <c r="B24" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C24">
         <v>23</v>
       </c>
       <c r="D24" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E24" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F24" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -2328,19 +2333,19 @@
         <v>78</v>
       </c>
       <c r="B25" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C25">
         <v>24</v>
       </c>
       <c r="D25" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E25" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F25" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -2348,19 +2353,19 @@
         <v>78</v>
       </c>
       <c r="B26" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C26">
         <v>25</v>
       </c>
       <c r="D26" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E26" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F26" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -2368,19 +2373,19 @@
         <v>78</v>
       </c>
       <c r="B27" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C27">
         <v>26</v>
       </c>
       <c r="D27" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E27" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F27" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -2388,19 +2393,19 @@
         <v>78</v>
       </c>
       <c r="B28" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C28">
         <v>27</v>
       </c>
       <c r="D28" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E28" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F28" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -2408,19 +2413,19 @@
         <v>78</v>
       </c>
       <c r="B29" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C29">
         <v>28</v>
       </c>
       <c r="D29" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E29" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F29" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -2428,19 +2433,19 @@
         <v>78</v>
       </c>
       <c r="B30" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C30">
         <v>29</v>
       </c>
       <c r="D30" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E30" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F30" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -2448,19 +2453,19 @@
         <v>78</v>
       </c>
       <c r="B31" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C31">
         <v>30</v>
       </c>
       <c r="D31" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E31" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F31" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -2468,19 +2473,19 @@
         <v>78</v>
       </c>
       <c r="B32" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C32">
         <v>31</v>
       </c>
       <c r="D32" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E32" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F32" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -2488,19 +2493,19 @@
         <v>78</v>
       </c>
       <c r="B33" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C33">
         <v>32</v>
       </c>
       <c r="D33" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E33" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F33" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -2508,19 +2513,19 @@
         <v>78</v>
       </c>
       <c r="B34" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C34">
         <v>33</v>
       </c>
       <c r="D34" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E34" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F34" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -2528,19 +2533,19 @@
         <v>78</v>
       </c>
       <c r="B35" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C35">
         <v>34</v>
       </c>
       <c r="D35" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E35" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F35" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -2548,19 +2553,19 @@
         <v>78</v>
       </c>
       <c r="B36" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C36">
         <v>35</v>
       </c>
       <c r="D36" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E36" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F36" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -2568,19 +2573,19 @@
         <v>78</v>
       </c>
       <c r="B37" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C37">
         <v>36</v>
       </c>
       <c r="D37" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E37" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F37" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -2588,19 +2593,19 @@
         <v>78</v>
       </c>
       <c r="B38" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C38">
         <v>37</v>
       </c>
       <c r="D38" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E38" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F38" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -2608,19 +2613,19 @@
         <v>78</v>
       </c>
       <c r="B39" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C39">
         <v>38</v>
       </c>
       <c r="D39" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E39" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F39" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -2628,19 +2633,19 @@
         <v>78</v>
       </c>
       <c r="B40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C40">
         <v>39</v>
       </c>
       <c r="D40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -2648,19 +2653,19 @@
         <v>78</v>
       </c>
       <c r="B41" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C41">
         <v>40</v>
       </c>
       <c r="D41" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E41" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F41" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -2668,19 +2673,19 @@
         <v>78</v>
       </c>
       <c r="B42" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C42">
         <v>41</v>
       </c>
       <c r="D42" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E42" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F42" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -2688,19 +2693,19 @@
         <v>78</v>
       </c>
       <c r="B43" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C43">
         <v>42</v>
       </c>
       <c r="D43" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E43" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F43" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -2708,19 +2713,19 @@
         <v>78</v>
       </c>
       <c r="B44" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C44">
         <v>43</v>
       </c>
       <c r="D44" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E44" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F44" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -2728,19 +2733,19 @@
         <v>78</v>
       </c>
       <c r="B45" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C45">
         <v>44</v>
       </c>
       <c r="D45" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E45" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F45" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -2748,19 +2753,19 @@
         <v>78</v>
       </c>
       <c r="B46" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C46">
         <v>45</v>
       </c>
       <c r="D46" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E46" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F46" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -2768,19 +2773,19 @@
         <v>78</v>
       </c>
       <c r="B47" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C47">
         <v>46</v>
       </c>
       <c r="D47" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E47" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F47" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -2788,19 +2793,19 @@
         <v>78</v>
       </c>
       <c r="B48" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C48">
         <v>47</v>
       </c>
       <c r="D48" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E48" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F48" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -2808,19 +2813,19 @@
         <v>78</v>
       </c>
       <c r="B49" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C49">
         <v>48</v>
       </c>
       <c r="D49" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E49" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F49" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -2828,19 +2833,19 @@
         <v>78</v>
       </c>
       <c r="B50" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C50">
         <v>49</v>
       </c>
       <c r="D50" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E50" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F50" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -2848,19 +2853,19 @@
         <v>78</v>
       </c>
       <c r="B51" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C51">
         <v>50</v>
       </c>
       <c r="D51" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E51" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F51" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -2868,19 +2873,19 @@
         <v>78</v>
       </c>
       <c r="B52" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C52">
         <v>51</v>
       </c>
       <c r="D52" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E52" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F52" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -2888,19 +2893,19 @@
         <v>78</v>
       </c>
       <c r="B53" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C53">
         <v>52</v>
       </c>
       <c r="D53" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E53" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F53" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -2908,19 +2913,19 @@
         <v>78</v>
       </c>
       <c r="B54" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C54">
         <v>53</v>
       </c>
       <c r="D54" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E54" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F54" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -2928,19 +2933,19 @@
         <v>78</v>
       </c>
       <c r="B55" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C55">
         <v>54</v>
       </c>
       <c r="D55" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E55" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F55" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -2948,19 +2953,19 @@
         <v>78</v>
       </c>
       <c r="B56" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C56">
         <v>55</v>
       </c>
       <c r="D56" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E56" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F56" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -2968,19 +2973,19 @@
         <v>78</v>
       </c>
       <c r="B57" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C57">
         <v>56</v>
       </c>
       <c r="D57" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E57" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F57" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -2988,19 +2993,19 @@
         <v>78</v>
       </c>
       <c r="B58" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C58">
         <v>57</v>
       </c>
       <c r="D58" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E58" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F58" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -3008,19 +3013,19 @@
         <v>78</v>
       </c>
       <c r="B59" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C59">
         <v>58</v>
       </c>
       <c r="D59" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E59" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F59" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -3028,19 +3033,19 @@
         <v>78</v>
       </c>
       <c r="B60" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C60">
         <v>59</v>
       </c>
       <c r="D60" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E60" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F60" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
@@ -3048,19 +3053,19 @@
         <v>78</v>
       </c>
       <c r="B61" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C61">
         <v>60</v>
       </c>
       <c r="D61" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E61" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F61" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
@@ -3068,19 +3073,19 @@
         <v>78</v>
       </c>
       <c r="B62" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C62">
         <v>61</v>
       </c>
       <c r="D62" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E62" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F62" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
@@ -3088,19 +3093,19 @@
         <v>78</v>
       </c>
       <c r="B63" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C63">
         <v>62</v>
       </c>
       <c r="D63" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E63" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F63" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -3108,19 +3113,19 @@
         <v>78</v>
       </c>
       <c r="B64" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C64">
         <v>63</v>
       </c>
       <c r="D64" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E64" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F64" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -3128,19 +3133,19 @@
         <v>78</v>
       </c>
       <c r="B65" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C65">
         <v>64</v>
       </c>
       <c r="D65" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E65" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F65" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -3148,19 +3153,19 @@
         <v>78</v>
       </c>
       <c r="B66" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C66">
         <v>65</v>
       </c>
       <c r="D66" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E66" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F66" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -3168,19 +3173,19 @@
         <v>78</v>
       </c>
       <c r="B67" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C67">
         <v>66</v>
       </c>
       <c r="D67" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E67" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F67" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -3188,19 +3193,19 @@
         <v>78</v>
       </c>
       <c r="B68" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C68">
         <v>67</v>
       </c>
       <c r="D68" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E68" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F68" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -3208,19 +3213,19 @@
         <v>78</v>
       </c>
       <c r="B69" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C69">
         <v>68</v>
       </c>
       <c r="D69" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E69" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F69" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -3228,19 +3233,19 @@
         <v>78</v>
       </c>
       <c r="B70" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C70">
         <v>69</v>
       </c>
       <c r="D70" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E70" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F70" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
@@ -3248,19 +3253,19 @@
         <v>78</v>
       </c>
       <c r="B71" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C71">
         <v>70</v>
       </c>
       <c r="D71" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E71" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F71" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
@@ -3268,19 +3273,19 @@
         <v>78</v>
       </c>
       <c r="B72" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C72">
         <v>71</v>
       </c>
       <c r="D72" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E72" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F72" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
@@ -3288,19 +3293,19 @@
         <v>78</v>
       </c>
       <c r="B73" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C73">
         <v>72</v>
       </c>
       <c r="D73" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E73" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F73" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
@@ -3308,19 +3313,19 @@
         <v>78</v>
       </c>
       <c r="B74" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C74">
         <v>73</v>
       </c>
       <c r="D74" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E74" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F74" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
@@ -3328,19 +3333,19 @@
         <v>78</v>
       </c>
       <c r="B75" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C75">
         <v>74</v>
       </c>
       <c r="D75" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E75" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F75" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
@@ -3348,19 +3353,19 @@
         <v>78</v>
       </c>
       <c r="B76" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C76">
         <v>75</v>
       </c>
       <c r="D76" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E76" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F76" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
@@ -3368,19 +3373,19 @@
         <v>78</v>
       </c>
       <c r="B77" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C77">
         <v>76</v>
       </c>
       <c r="D77" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E77" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F77" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
@@ -3388,19 +3393,19 @@
         <v>78</v>
       </c>
       <c r="B78" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C78">
         <v>77</v>
       </c>
       <c r="D78" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E78" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F78" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -3408,19 +3413,19 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C79">
         <v>78</v>
       </c>
       <c r="D79" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E79" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F79" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -3428,19 +3433,19 @@
         <v>78</v>
       </c>
       <c r="B80" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C80">
         <v>79</v>
       </c>
       <c r="D80" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E80" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F80" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
@@ -3448,19 +3453,19 @@
         <v>78</v>
       </c>
       <c r="B81" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C81">
         <v>80</v>
       </c>
       <c r="D81" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E81" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F81" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
@@ -3468,19 +3473,19 @@
         <v>78</v>
       </c>
       <c r="B82" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C82">
         <v>81</v>
       </c>
       <c r="D82" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E82" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F82" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
@@ -3488,19 +3493,19 @@
         <v>78</v>
       </c>
       <c r="B83" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C83">
         <v>82</v>
       </c>
       <c r="D83" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E83" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F83" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -3508,19 +3513,19 @@
         <v>78</v>
       </c>
       <c r="B84" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C84">
         <v>83</v>
       </c>
       <c r="D84" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E84" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F84" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -3528,19 +3533,19 @@
         <v>78</v>
       </c>
       <c r="B85" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C85">
         <v>84</v>
       </c>
       <c r="D85" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E85" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F85" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -3548,19 +3553,19 @@
         <v>78</v>
       </c>
       <c r="B86" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C86">
         <v>85</v>
       </c>
       <c r="D86" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E86" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F86" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
@@ -3568,19 +3573,19 @@
         <v>78</v>
       </c>
       <c r="B87" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C87">
         <v>86</v>
       </c>
       <c r="D87" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E87" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F87" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -3588,19 +3593,19 @@
         <v>78</v>
       </c>
       <c r="B88" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C88">
         <v>87</v>
       </c>
       <c r="D88" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E88" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F88" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
@@ -3608,19 +3613,19 @@
         <v>78</v>
       </c>
       <c r="B89" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C89">
         <v>88</v>
       </c>
       <c r="D89" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E89" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F89" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
@@ -3628,19 +3633,19 @@
         <v>78</v>
       </c>
       <c r="B90" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C90">
         <v>89</v>
       </c>
       <c r="D90" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E90" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F90" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
@@ -3648,19 +3653,19 @@
         <v>78</v>
       </c>
       <c r="B91" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C91">
         <v>90</v>
       </c>
       <c r="D91" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E91" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F91" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
@@ -3668,19 +3673,19 @@
         <v>78</v>
       </c>
       <c r="B92" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C92">
         <v>91</v>
       </c>
       <c r="D92" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E92" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F92" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
@@ -3688,19 +3693,19 @@
         <v>78</v>
       </c>
       <c r="B93" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C93">
         <v>92</v>
       </c>
       <c r="D93" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E93" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F93" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
@@ -3708,19 +3713,19 @@
         <v>78</v>
       </c>
       <c r="B94" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C94">
         <v>93</v>
       </c>
       <c r="D94" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E94" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F94" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
@@ -3728,19 +3733,19 @@
         <v>78</v>
       </c>
       <c r="B95" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C95">
         <v>94</v>
       </c>
       <c r="D95" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E95" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F95" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
@@ -3748,19 +3753,19 @@
         <v>78</v>
       </c>
       <c r="B96" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C96">
         <v>95</v>
       </c>
       <c r="D96" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E96" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F96" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
@@ -3768,19 +3773,19 @@
         <v>78</v>
       </c>
       <c r="B97" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C97">
         <v>96</v>
       </c>
       <c r="D97" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E97" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F97" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
@@ -3788,19 +3793,19 @@
         <v>78</v>
       </c>
       <c r="B98" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C98">
         <v>97</v>
       </c>
       <c r="D98" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E98" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F98" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
@@ -3808,19 +3813,19 @@
         <v>85</v>
       </c>
       <c r="B99" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C99">
         <v>1</v>
       </c>
       <c r="D99" t="s">
+        <v>222</v>
+      </c>
+      <c r="E99" t="s">
         <v>223</v>
       </c>
-      <c r="E99" t="s">
+      <c r="F99" t="s">
         <v>224</v>
-      </c>
-      <c r="F99" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
@@ -3828,7 +3833,7 @@
         <v>85</v>
       </c>
       <c r="B100" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C100">
         <v>2</v>
@@ -3848,22 +3853,22 @@
         <v>92</v>
       </c>
       <c r="B101" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C101">
         <v>1</v>
       </c>
       <c r="D101" t="s">
+        <v>227</v>
+      </c>
+      <c r="E101" t="s">
         <v>228</v>
       </c>
-      <c r="E101" t="s">
+      <c r="F101" t="s">
         <v>229</v>
       </c>
-      <c r="F101" t="s">
-        <v>230</v>
-      </c>
       <c r="G101" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
@@ -3871,22 +3876,22 @@
         <v>92</v>
       </c>
       <c r="B102" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C102">
         <v>2</v>
       </c>
       <c r="D102" t="s">
+        <v>231</v>
+      </c>
+      <c r="E102" t="s">
         <v>232</v>
       </c>
-      <c r="E102" t="s">
+      <c r="F102" t="s">
         <v>233</v>
       </c>
-      <c r="F102" t="s">
-        <v>234</v>
-      </c>
       <c r="G102" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
@@ -3894,19 +3899,19 @@
         <v>92</v>
       </c>
       <c r="B103" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C103">
         <v>3</v>
       </c>
       <c r="D103" t="s">
+        <v>235</v>
+      </c>
+      <c r="E103" t="s">
         <v>236</v>
       </c>
-      <c r="E103" t="s">
+      <c r="F103" t="s">
         <v>237</v>
-      </c>
-      <c r="F103" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
@@ -3914,7 +3919,7 @@
         <v>92</v>
       </c>
       <c r="B104" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C104">
         <v>4</v>
@@ -3929,7 +3934,7 @@
         <v>97</v>
       </c>
       <c r="G104" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
@@ -3937,19 +3942,19 @@
         <v>98</v>
       </c>
       <c r="B105" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C105">
         <v>1</v>
       </c>
       <c r="D105" t="s">
+        <v>240</v>
+      </c>
+      <c r="E105" t="s">
         <v>241</v>
       </c>
-      <c r="E105" t="s">
+      <c r="F105" t="s">
         <v>242</v>
-      </c>
-      <c r="F105" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
@@ -3957,19 +3962,19 @@
         <v>98</v>
       </c>
       <c r="B106" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C106">
         <v>2</v>
       </c>
       <c r="D106" t="s">
+        <v>244</v>
+      </c>
+      <c r="E106" t="s">
         <v>245</v>
       </c>
-      <c r="E106" t="s">
+      <c r="F106" t="s">
         <v>246</v>
-      </c>
-      <c r="F106" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
@@ -3977,7 +3982,7 @@
         <v>98</v>
       </c>
       <c r="B107" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C107">
         <v>3</v>
@@ -3997,7 +4002,7 @@
         <v>105</v>
       </c>
       <c r="B108" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C108">
         <v>1</v>
@@ -4017,19 +4022,19 @@
         <v>105</v>
       </c>
       <c r="B109" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C109">
         <v>2</v>
       </c>
       <c r="D109" t="s">
+        <v>250</v>
+      </c>
+      <c r="E109" t="s">
         <v>251</v>
       </c>
-      <c r="E109" t="s">
+      <c r="F109" t="s">
         <v>252</v>
-      </c>
-      <c r="F109" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
@@ -4037,7 +4042,7 @@
         <v>110</v>
       </c>
       <c r="B110" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C110">
         <v>1</v>
@@ -4057,19 +4062,19 @@
         <v>110</v>
       </c>
       <c r="B111" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C111">
         <v>2</v>
       </c>
       <c r="D111" t="s">
+        <v>254</v>
+      </c>
+      <c r="E111" t="s">
         <v>255</v>
       </c>
-      <c r="E111" t="s">
+      <c r="F111" t="s">
         <v>256</v>
-      </c>
-      <c r="F111" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
@@ -4077,19 +4082,19 @@
         <v>110</v>
       </c>
       <c r="B112" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C112">
         <v>3</v>
       </c>
       <c r="D112" t="s">
+        <v>258</v>
+      </c>
+      <c r="E112" t="s">
         <v>259</v>
       </c>
-      <c r="E112" t="s">
+      <c r="F112" t="s">
         <v>260</v>
-      </c>
-      <c r="F112" t="s">
-        <v>261</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Make elimination language independent
Close #406
</commit_message>
<xml_diff>
--- a/tests/testthat/fixtures/metadata/metadata_BEXLTALL.xlsx
+++ b/tests/testthat/fixtures/metadata/metadata_BEXLTALL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johan Ejstrud\Dropbox\repo\pxmake\tests\testthat\fixtures\metadata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johan\Dropbox\repo\pxmake\tests\testthat\fixtures\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E530AFCA-C9C2-49D5-BFD5-6062E5C8692F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7469944A-3B3E-46D1-9B0E-F085F6CF5BDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19005" yWindow="3960" windowWidth="15450" windowHeight="13425" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14985" yWindow="0" windowWidth="24690" windowHeight="31785" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="261">
   <si>
     <t>keyword</t>
   </si>
@@ -238,15 +238,6 @@
     <t>kl_domain</t>
   </si>
   <si>
-    <t>en_elimination</t>
-  </si>
-  <si>
-    <t>da_elimination</t>
-  </si>
-  <si>
-    <t>kl_elimination</t>
-  </si>
-  <si>
     <t>en_note</t>
   </si>
   <si>
@@ -812,6 +803,9 @@
   </si>
   <si>
     <t>timeval</t>
+  </si>
+  <si>
+    <t>elimination</t>
   </si>
 </sst>
 </file>
@@ -892,23 +886,21 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table5" displayName="Table5" ref="A1:Q9" totalsRowShown="0">
-  <autoFilter ref="A1:Q9" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
-  <tableColumns count="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table5" displayName="Table5" ref="A1:O9" totalsRowShown="0">
+  <autoFilter ref="A1:O9" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
+  <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="pivot"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="order"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="variable-code"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="variable-type"/>
     <tableColumn id="17" xr3:uid="{1F674A62-667E-4B54-9697-04C2424B310A}" name="timeval"/>
+    <tableColumn id="18" xr3:uid="{0B451380-3DAB-47FC-BBC4-86BCBE0FB4E6}" name="elimination"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="en_variable-label"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="da_variable-label"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="kl_variable-label"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="en_domain"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="da_domain"/>
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="kl_domain"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="en_elimination"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="da_elimination"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0200-00000D000000}" name="kl_elimination"/>
     <tableColumn id="14" xr3:uid="{00000000-0010-0000-0200-00000E000000}" name="en_note"/>
     <tableColumn id="15" xr3:uid="{00000000-0010-0000-0200-00000F000000}" name="da_note"/>
     <tableColumn id="16" xr3:uid="{00000000-0010-0000-0200-000010000000}" name="kl_note"/>
@@ -1514,10 +1506,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Q9"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1527,21 +1519,19 @@
     <col min="3" max="3" width="15.5703125" customWidth="1"/>
     <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.28515625" customWidth="1"/>
-    <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" customWidth="1"/>
+    <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>62</v>
       </c>
@@ -1552,269 +1542,227 @@
         <v>64</v>
       </c>
       <c r="D1" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="E1" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F1" t="s">
+        <v>260</v>
+      </c>
+      <c r="G1" t="s">
         <v>65</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>66</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>67</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>68</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>69</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>70</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>71</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>72</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>73</v>
       </c>
-      <c r="O1" t="s">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>74</v>
-      </c>
-      <c r="P1" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>77</v>
       </c>
       <c r="B2">
         <v>5</v>
       </c>
       <c r="C2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F2" t="s">
+        <v>81</v>
+      </c>
+      <c r="G2" t="s">
+        <v>75</v>
+      </c>
+      <c r="H2" t="s">
+        <v>76</v>
+      </c>
+      <c r="I2" t="s">
+        <v>77</v>
+      </c>
+      <c r="J2" t="s">
         <v>78</v>
       </c>
-      <c r="F2" t="s">
-        <v>78</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="K2" t="s">
         <v>79</v>
       </c>
-      <c r="H2" t="s">
+      <c r="L2" t="s">
         <v>80</v>
       </c>
-      <c r="I2" t="s">
-        <v>81</v>
-      </c>
-      <c r="J2" t="s">
-        <v>82</v>
-      </c>
-      <c r="K2" t="s">
-        <v>83</v>
-      </c>
-      <c r="L2" t="s">
-        <v>84</v>
-      </c>
-      <c r="M2" t="s">
-        <v>84</v>
-      </c>
-      <c r="N2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F3" t="s">
+        <v>222</v>
+      </c>
+      <c r="G3" t="s">
+        <v>83</v>
+      </c>
+      <c r="H3" t="s">
+        <v>84</v>
+      </c>
+      <c r="I3" t="s">
         <v>85</v>
       </c>
-      <c r="F3" t="s">
-        <v>86</v>
-      </c>
-      <c r="G3" t="s">
-        <v>87</v>
-      </c>
-      <c r="H3" t="s">
-        <v>88</v>
-      </c>
-      <c r="L3" t="s">
-        <v>89</v>
-      </c>
-      <c r="M3" t="s">
-        <v>90</v>
-      </c>
-      <c r="N3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B4">
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F4" t="s">
-        <v>92</v>
+        <v>235</v>
       </c>
       <c r="G4" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="H4" t="s">
-        <v>94</v>
-      </c>
-      <c r="L4" t="s">
-        <v>95</v>
-      </c>
-      <c r="M4" t="s">
-        <v>96</v>
-      </c>
-      <c r="N4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+      <c r="I4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B5">
         <v>2</v>
       </c>
       <c r="C5" t="s">
+        <v>95</v>
+      </c>
+      <c r="F5" t="s">
+        <v>244</v>
+      </c>
+      <c r="G5" t="s">
+        <v>96</v>
+      </c>
+      <c r="H5" t="s">
+        <v>97</v>
+      </c>
+      <c r="I5" t="s">
         <v>98</v>
       </c>
-      <c r="F5" t="s">
-        <v>99</v>
-      </c>
-      <c r="G5" t="s">
-        <v>100</v>
-      </c>
-      <c r="H5" t="s">
-        <v>101</v>
-      </c>
-      <c r="L5" t="s">
-        <v>102</v>
-      </c>
-      <c r="M5" t="s">
-        <v>103</v>
-      </c>
-      <c r="N5" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B6">
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F6" t="s">
-        <v>105</v>
+        <v>245</v>
       </c>
       <c r="G6" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="H6" t="s">
-        <v>107</v>
-      </c>
-      <c r="L6" t="s">
-        <v>108</v>
-      </c>
-      <c r="M6" t="s">
-        <v>108</v>
-      </c>
-      <c r="N6" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+      <c r="I6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B7">
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F7" t="s">
-        <v>110</v>
+        <v>245</v>
       </c>
       <c r="G7" t="s">
+        <v>107</v>
+      </c>
+      <c r="H7" t="s">
+        <v>108</v>
+      </c>
+      <c r="I7" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>111</v>
-      </c>
-      <c r="H7" t="s">
-        <v>112</v>
-      </c>
-      <c r="L7" t="s">
-        <v>108</v>
-      </c>
-      <c r="M7" t="s">
-        <v>113</v>
-      </c>
-      <c r="N7" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>114</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E8" t="b">
         <v>1</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
+        <v>112</v>
+      </c>
+      <c r="H8" t="s">
+        <v>113</v>
+      </c>
+      <c r="I8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>115</v>
-      </c>
-      <c r="G8" t="s">
-        <v>116</v>
-      </c>
-      <c r="H8" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>118</v>
       </c>
       <c r="C9" t="s">
         <v>1</v>
       </c>
-      <c r="F9" t="s">
-        <v>119</v>
-      </c>
       <c r="G9" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="H9" t="s">
-        <v>120</v>
+        <v>116</v>
+      </c>
+      <c r="I9" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -1830,8 +1778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G112"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView showGridLines="0" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="B110" sqref="B110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1853,24 +1801,24 @@
         <v>24</v>
       </c>
       <c r="C1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F1" t="s">
         <v>121</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>122</v>
-      </c>
-      <c r="E1" t="s">
-        <v>123</v>
-      </c>
-      <c r="F1" t="s">
-        <v>124</v>
-      </c>
-      <c r="G1" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B2" t="s">
         <v>19</v>
@@ -1890,287 +1838,287 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B4" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E4" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="F4" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B5" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E5" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F5" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="F6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B7" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C7">
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E7" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F7" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B8" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C8">
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E8" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F8" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B9" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C9">
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E9" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F9" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B10" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C10">
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E10" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F10" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B11" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C11">
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E11" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F11" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B12" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C12">
         <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E12" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F12" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B13" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C13">
         <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E13" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F13" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B14" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C14">
         <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E14" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="F14" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B15" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C15">
         <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E15" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F15" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B16" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C16">
         <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E16" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="F16" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B17" t="s">
         <v>17</v>
@@ -2190,1911 +2138,1911 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B18" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C18">
         <v>17</v>
       </c>
       <c r="D18" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E18" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="F18" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B19" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C19">
         <v>18</v>
       </c>
       <c r="D19" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E19" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F19" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B20" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C20">
         <v>19</v>
       </c>
       <c r="D20" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E20" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F20" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B21" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C21">
         <v>20</v>
       </c>
       <c r="D21" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E21" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F21" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B22" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C22">
         <v>21</v>
       </c>
       <c r="D22" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E22" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F22" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B23" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C23">
         <v>22</v>
       </c>
       <c r="D23" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E23" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="F23" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B24" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C24">
         <v>23</v>
       </c>
       <c r="D24" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E24" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F24" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B25" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C25">
         <v>24</v>
       </c>
       <c r="D25" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E25" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F25" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B26" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C26">
         <v>25</v>
       </c>
       <c r="D26" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E26" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="F26" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B27" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C27">
         <v>26</v>
       </c>
       <c r="D27" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E27" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F27" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B28" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C28">
         <v>27</v>
       </c>
       <c r="D28" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E28" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F28" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B29" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C29">
         <v>28</v>
       </c>
       <c r="D29" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E29" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="F29" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B30" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C30">
         <v>29</v>
       </c>
       <c r="D30" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E30" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F30" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B31" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C31">
         <v>30</v>
       </c>
       <c r="D31" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E31" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F31" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B32" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C32">
         <v>31</v>
       </c>
       <c r="D32" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E32" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F32" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B33" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C33">
         <v>32</v>
       </c>
       <c r="D33" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E33" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="F33" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B34" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C34">
         <v>33</v>
       </c>
       <c r="D34" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E34" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="F34" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B35" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C35">
         <v>34</v>
       </c>
       <c r="D35" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E35" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="F35" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B36" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C36">
         <v>35</v>
       </c>
       <c r="D36" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E36" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F36" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B37" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C37">
         <v>36</v>
       </c>
       <c r="D37" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E37" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="F37" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B38" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C38">
         <v>37</v>
       </c>
       <c r="D38" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E38" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="F38" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B39" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C39">
         <v>38</v>
       </c>
       <c r="D39" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E39" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F39" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B40" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C40">
         <v>39</v>
       </c>
       <c r="D40" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E40" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F40" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B41" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C41">
         <v>40</v>
       </c>
       <c r="D41" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E41" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="F41" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B42" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C42">
         <v>41</v>
       </c>
       <c r="D42" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E42" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="F42" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B43" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C43">
         <v>42</v>
       </c>
       <c r="D43" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E43" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="F43" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B44" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C44">
         <v>43</v>
       </c>
       <c r="D44" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E44" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="F44" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B45" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C45">
         <v>44</v>
       </c>
       <c r="D45" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E45" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="F45" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B46" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C46">
         <v>45</v>
       </c>
       <c r="D46" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E46" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="F46" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B47" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C47">
         <v>46</v>
       </c>
       <c r="D47" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E47" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F47" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B48" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C48">
         <v>47</v>
       </c>
       <c r="D48" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="E48" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F48" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B49" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C49">
         <v>48</v>
       </c>
       <c r="D49" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="E49" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="F49" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B50" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C50">
         <v>49</v>
       </c>
       <c r="D50" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E50" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F50" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B51" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C51">
         <v>50</v>
       </c>
       <c r="D51" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E51" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="F51" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B52" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C52">
         <v>51</v>
       </c>
       <c r="D52" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="E52" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="F52" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B53" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C53">
         <v>52</v>
       </c>
       <c r="D53" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E53" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="F53" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B54" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C54">
         <v>53</v>
       </c>
       <c r="D54" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E54" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="F54" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B55" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C55">
         <v>54</v>
       </c>
       <c r="D55" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E55" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="F55" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B56" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C56">
         <v>55</v>
       </c>
       <c r="D56" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E56" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="F56" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B57" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C57">
         <v>56</v>
       </c>
       <c r="D57" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E57" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="F57" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B58" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C58">
         <v>57</v>
       </c>
       <c r="D58" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="E58" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F58" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B59" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C59">
         <v>58</v>
       </c>
       <c r="D59" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E59" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F59" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B60" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C60">
         <v>59</v>
       </c>
       <c r="D60" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E60" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="F60" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B61" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C61">
         <v>60</v>
       </c>
       <c r="D61" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E61" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="F61" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B62" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C62">
         <v>61</v>
       </c>
       <c r="D62" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E62" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="F62" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B63" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C63">
         <v>62</v>
       </c>
       <c r="D63" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E63" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="F63" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B64" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C64">
         <v>63</v>
       </c>
       <c r="D64" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="E64" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="F64" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B65" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C65">
         <v>64</v>
       </c>
       <c r="D65" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E65" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="F65" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B66" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C66">
         <v>65</v>
       </c>
       <c r="D66" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E66" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="F66" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B67" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C67">
         <v>66</v>
       </c>
       <c r="D67" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="E67" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F67" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B68" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C68">
         <v>67</v>
       </c>
       <c r="D68" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E68" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="F68" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B69" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C69">
         <v>68</v>
       </c>
       <c r="D69" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E69" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="F69" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B70" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C70">
         <v>69</v>
       </c>
       <c r="D70" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E70" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="F70" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B71" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C71">
         <v>70</v>
       </c>
       <c r="D71" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E71" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="F71" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B72" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C72">
         <v>71</v>
       </c>
       <c r="D72" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="E72" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="F72" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B73" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C73">
         <v>72</v>
       </c>
       <c r="D73" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="E73" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F73" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B74" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C74">
         <v>73</v>
       </c>
       <c r="D74" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="E74" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="F74" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B75" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C75">
         <v>74</v>
       </c>
       <c r="D75" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="E75" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="F75" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C76">
         <v>75</v>
       </c>
       <c r="D76" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E76" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="F76" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B77" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C77">
         <v>76</v>
       </c>
       <c r="D77" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E77" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="F77" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B78" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C78">
         <v>77</v>
       </c>
       <c r="D78" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E78" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="F78" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B79" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C79">
         <v>78</v>
       </c>
       <c r="D79" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E79" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="F79" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B80" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C80">
         <v>79</v>
       </c>
       <c r="D80" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E80" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="F80" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B81" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C81">
         <v>80</v>
       </c>
       <c r="D81" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="E81" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="F81" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B82" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C82">
         <v>81</v>
       </c>
       <c r="D82" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E82" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="F82" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B83" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C83">
         <v>82</v>
       </c>
       <c r="D83" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E83" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="F83" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B84" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C84">
         <v>83</v>
       </c>
       <c r="D84" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E84" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="F84" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B85" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C85">
         <v>84</v>
       </c>
       <c r="D85" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E85" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="F85" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B86" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C86">
         <v>85</v>
       </c>
       <c r="D86" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E86" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="F86" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B87" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C87">
         <v>86</v>
       </c>
       <c r="D87" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E87" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="F87" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B88" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C88">
         <v>87</v>
       </c>
       <c r="D88" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="E88" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="F88" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B89" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C89">
         <v>88</v>
       </c>
       <c r="D89" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="E89" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="F89" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B90" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C90">
         <v>89</v>
       </c>
       <c r="D90" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="E90" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F90" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B91" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C91">
         <v>90</v>
       </c>
       <c r="D91" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="E91" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="F91" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B92" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C92">
         <v>91</v>
       </c>
       <c r="D92" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="E92" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="F92" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B93" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C93">
         <v>92</v>
       </c>
       <c r="D93" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="E93" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="F93" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B94" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C94">
         <v>93</v>
       </c>
       <c r="D94" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="E94" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="F94" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B95" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C95">
         <v>94</v>
       </c>
       <c r="D95" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="E95" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="F95" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B96" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C96">
         <v>95</v>
       </c>
       <c r="D96" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="E96" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="F96" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B97" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C97">
         <v>96</v>
       </c>
       <c r="D97" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="E97" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="F97" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B98" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C98">
         <v>97</v>
       </c>
       <c r="D98" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="E98" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="F98" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B99" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C99">
         <v>1</v>
       </c>
       <c r="D99" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="E99" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="F99" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B100" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C100">
         <v>2</v>
       </c>
       <c r="D100" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E100" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F100" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B101" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C101">
         <v>1</v>
       </c>
       <c r="D101" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="E101" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="F101" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="G101" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B102" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C102">
         <v>2</v>
       </c>
       <c r="D102" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="E102" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="F102" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="G102" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B103" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C103">
         <v>3</v>
       </c>
       <c r="D103" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="E103" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="F103" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B104" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C104">
         <v>4</v>
       </c>
       <c r="D104" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E104" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F104" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G104" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B105" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C105">
         <v>1</v>
       </c>
       <c r="D105" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="E105" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="F105" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B106" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C106">
         <v>2</v>
       </c>
       <c r="D106" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="E106" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="F106" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B107" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C107">
         <v>3</v>
       </c>
       <c r="D107" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E107" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F107" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B108" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C108">
         <v>1</v>
       </c>
       <c r="D108" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E108" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="F108" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B109" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C109">
         <v>2</v>
       </c>
       <c r="D109" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="E109" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="F109" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B110" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C110">
         <v>1</v>
       </c>
       <c r="D110" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E110" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F110" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B111" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C111">
         <v>2</v>
       </c>
       <c r="D111" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="E111" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="F111" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B112" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C112">
         <v>3</v>
       </c>
       <c r="D112" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="E112" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="F112" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
   </sheetData>

</xml_diff>